<commit_message>
data update, including first no2- data
</commit_message>
<xml_diff>
--- a/data/exp_raw/ssexp_data.xlsx
+++ b/data/exp_raw/ssexp_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vcantarella/Documents/FuhrbergerColumns/data/exp_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF13E4D-269A-2B42-BA38-952C520B1A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BBF40B-AB9E-A84B-A02E-54BDD392B269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16680" activeTab="3" xr2:uid="{82067E57-95C1-4A4D-B858-7597035F15DE}"/>
+    <workbookView xWindow="620" yWindow="800" windowWidth="28040" windowHeight="16680" activeTab="3" xr2:uid="{82067E57-95C1-4A4D-B858-7597035F15DE}"/>
   </bookViews>
   <sheets>
     <sheet name="general_samples_p1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,12 @@
     <sheet name="general_samples_p4" sheetId="6" r:id="rId4"/>
     <sheet name="fe" sheetId="2" r:id="rId5"/>
     <sheet name="hs" sheetId="3" r:id="rId6"/>
+    <sheet name="standard_curve_no2" sheetId="7" r:id="rId7"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="190">
   <si>
     <t>Sample</t>
   </si>
@@ -533,13 +538,91 @@
   </si>
   <si>
     <t>* volume sample interrupted because of Fe sampling</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>column/batch</t>
+  </si>
+  <si>
+    <t>val1</t>
+  </si>
+  <si>
+    <t>dil</t>
+  </si>
+  <si>
+    <t>no2- [micromol/L]</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Value 1</t>
+  </si>
+  <si>
+    <t>Value 2</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>19-20B</t>
+  </si>
+  <si>
+    <t>13-14A</t>
+  </si>
+  <si>
+    <t>13-14B</t>
+  </si>
+  <si>
+    <t>17-18B</t>
+  </si>
+  <si>
+    <t>16-17B</t>
+  </si>
+  <si>
+    <t>17-18A</t>
+  </si>
+  <si>
+    <t>18-19</t>
+  </si>
+  <si>
+    <t>19-20A</t>
+  </si>
+  <si>
+    <t>16-17A</t>
+  </si>
+  <si>
+    <t>P1T0</t>
+  </si>
+  <si>
+    <t>P2T0</t>
+  </si>
+  <si>
+    <t>P3T0</t>
+  </si>
+  <si>
+    <t>P4T0</t>
+  </si>
+  <si>
+    <t>* cleaned pump tubing</t>
+  </si>
+  <si>
+    <t>* vial broke + cleaned pump tubing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -549,6 +632,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -574,9 +664,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,6 +683,1148 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>calibration range</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.8468522626868989E-2"/>
+                  <c:y val="-1.6007093312307215E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-DE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>standard_curve_no2!$J$2:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.59166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.34966666666666663</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.27066666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.6000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.6000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'[2]standard_curve_plate 2'!$H$2:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-088E-7F4D-9215-C1CC9BC3BE0C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1885324960"/>
+        <c:axId val="1885326672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1885324960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1885326672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1885326672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1885324960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>379240</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>50494</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07996E71-4B72-9647-A6A7-F60A119B0F97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="standard_curve_no2-test"/>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="J2">
+            <v>0.59166666666666667</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="J3">
+            <v>0.48500000000000004</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="J4">
+            <v>0.34966666666666663</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="J5">
+            <v>0.27066666666666667</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="J6">
+            <v>0.15166666666666667</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="J7">
+            <v>8.6000000000000007E-2</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="J8">
+            <v>4.6000000000000006E-2</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="J9">
+            <v>4.4999999999999998E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="standard_curve_plate_1"/>
+      <sheetName val="standard_curve_plate 2"/>
+      <sheetName val="standard_curve_plate_3"/>
+      <sheetName val="standard_curve_plate 4"/>
+      <sheetName val="fe_plate_1"/>
+      <sheetName val="br_standard_curve"/>
+      <sheetName val="sampling"/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="data"/>
+      <sheetName val="new_data"/>
+      <sheetName val="Sheet2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="2">
+          <cell r="H2">
+            <v>50</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="H3">
+            <v>40</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="H4">
+            <v>30</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="H5">
+            <v>20</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="H6">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="H7">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="H8">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -914,7 +2147,7 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -977,7 +2210,7 @@
         <v>18.91</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E24" si="0">(D2-6.75)/6</f>
+        <f t="shared" ref="E2:E28" si="0">(D2-6.75)/6</f>
         <v>2.0266666666666668</v>
       </c>
     </row>
@@ -1461,6 +2694,13 @@
         <f t="shared" si="2"/>
         <v>45928.71597222222</v>
       </c>
+      <c r="D25">
+        <v>18.350000000000001</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>1.9333333333333336</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -1474,6 +2714,13 @@
         <f t="shared" si="2"/>
         <v>45928.96597222222</v>
       </c>
+      <c r="D26">
+        <v>18.22</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>1.9116666666666664</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -1487,6 +2734,13 @@
         <f t="shared" si="2"/>
         <v>45929.21597222222</v>
       </c>
+      <c r="D27">
+        <v>18.29</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>1.9233333333333331</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -1499,6 +2753,25 @@
       <c r="C28" s="1">
         <f t="shared" si="2"/>
         <v>45929.46597222222</v>
+      </c>
+      <c r="D28">
+        <v>18.190000000000001</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>1.906666666666667</v>
+      </c>
+      <c r="F28">
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="G28">
+        <v>924</v>
+      </c>
+      <c r="H28">
+        <v>14.4</v>
+      </c>
+      <c r="L28" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -1616,7 +2889,7 @@
   <dimension ref="A1:L62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1677,7 +2950,7 @@
         <v>17.7</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E24" si="0">(D2-6.75)/6</f>
+        <f t="shared" ref="E2:E27" si="0">(D2-6.75)/6</f>
         <v>1.825</v>
       </c>
     </row>
@@ -2161,6 +3434,13 @@
         <f t="shared" si="2"/>
         <v>45928.71597222222</v>
       </c>
+      <c r="D25">
+        <v>19.48</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>2.1216666666666666</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -2174,6 +3454,13 @@
         <f t="shared" si="2"/>
         <v>45928.96597222222</v>
       </c>
+      <c r="D26">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>2.1083333333333329</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -2187,6 +3474,22 @@
         <f t="shared" si="2"/>
         <v>45929.21597222222</v>
       </c>
+      <c r="D27">
+        <v>19.63</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>2.1466666666666665</v>
+      </c>
+      <c r="F27">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="G27">
+        <v>846</v>
+      </c>
+      <c r="H27">
+        <v>13.3</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -2199,6 +3502,9 @@
       <c r="C28" s="1">
         <f t="shared" si="2"/>
         <v>45929.46597222222</v>
+      </c>
+      <c r="L28" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -2420,7 +3726,7 @@
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2481,7 +3787,7 @@
         <v>17.64</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E24" si="0">(D2-6.75)/6</f>
+        <f t="shared" ref="E2:E28" si="0">(D2-6.75)/6</f>
         <v>1.8150000000000002</v>
       </c>
     </row>
@@ -2965,6 +4271,13 @@
         <f t="shared" si="2"/>
         <v>45928.71597222222</v>
       </c>
+      <c r="D25">
+        <v>19.88</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>2.188333333333333</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -2978,6 +4291,13 @@
         <f t="shared" si="2"/>
         <v>45928.96597222222</v>
       </c>
+      <c r="D26">
+        <v>19.73</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>2.1633333333333336</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -2991,6 +4311,13 @@
         <f t="shared" si="2"/>
         <v>45929.21597222222</v>
       </c>
+      <c r="D27">
+        <v>19.77</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>2.17</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -3003,6 +4330,25 @@
       <c r="C28" s="1">
         <f t="shared" si="2"/>
         <v>45929.46597222222</v>
+      </c>
+      <c r="D28">
+        <v>19.89</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>2.19</v>
+      </c>
+      <c r="F28">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="G28">
+        <v>872</v>
+      </c>
+      <c r="H28">
+        <v>13.2</v>
+      </c>
+      <c r="L28" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -3180,7 +4526,7 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3241,7 +4587,7 @@
         <v>18.05</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E24" si="0">(D2-6.75)/6</f>
+        <f t="shared" ref="E2:E28" si="0">(D2-6.75)/6</f>
         <v>1.8833333333333335</v>
       </c>
     </row>
@@ -3725,6 +5071,13 @@
         <f t="shared" si="2"/>
         <v>45928.71597222222</v>
       </c>
+      <c r="D25">
+        <v>21.45</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>2.4499999999999997</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -3738,6 +5091,13 @@
         <f t="shared" si="2"/>
         <v>45928.96597222222</v>
       </c>
+      <c r="D26">
+        <v>21.28</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>2.4216666666666669</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -3751,6 +5111,13 @@
         <f t="shared" si="2"/>
         <v>45929.21597222222</v>
       </c>
+      <c r="D27">
+        <v>20.92</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>2.3616666666666668</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -3763,6 +5130,25 @@
       <c r="C28" s="1">
         <f t="shared" si="2"/>
         <v>45929.46597222222</v>
+      </c>
+      <c r="D28">
+        <v>20.99</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>2.3733333333333331</v>
+      </c>
+      <c r="F28">
+        <v>7.95</v>
+      </c>
+      <c r="G28">
+        <v>635</v>
+      </c>
+      <c r="H28">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L28" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -4035,4 +5421,750 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A1C8F7-0C5B-6045-992F-0FD6B0162923}">
+  <dimension ref="A1:J37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I1" t="s">
+        <v>171</v>
+      </c>
+      <c r="J1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>12.09</v>
+      </c>
+      <c r="B2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT("F",B2,"-",A2)</f>
+        <v>FP1-12.09</v>
+      </c>
+      <c r="D2">
+        <v>0.314</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F12" si="0">64.069*AVERAGE(D2:D2)-2.8707</f>
+        <v>17.246966</v>
+      </c>
+      <c r="G2">
+        <v>50</v>
+      </c>
+      <c r="H2">
+        <v>0.873</v>
+      </c>
+      <c r="I2">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ref="J2:J8" si="1">SUM(H2:I2)/3</f>
+        <v>0.59166666666666667</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>12.09</v>
+      </c>
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C13" si="2">_xlfn.CONCAT("F",B3,"-",A3)</f>
+        <v>Fcontrol-12.09</v>
+      </c>
+      <c r="D3">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>11.672963000000001</v>
+      </c>
+      <c r="G3">
+        <v>40</v>
+      </c>
+      <c r="H3">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="I3">
+        <v>0.74</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="1"/>
+        <v>0.48500000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>12.09</v>
+      </c>
+      <c r="B4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="2"/>
+        <v>F19-20B-12.09</v>
+      </c>
+      <c r="D4">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>10.263445000000001</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
+      <c r="H4">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="I4">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>0.34966666666666663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>12.09</v>
+      </c>
+      <c r="B5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="2"/>
+        <v>F13-14A-12.09</v>
+      </c>
+      <c r="D5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.90937100000000015</v>
+      </c>
+      <c r="G5">
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="I5">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>0.27066666666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>12.09</v>
+      </c>
+      <c r="B6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="2"/>
+        <v>F13-14B-12.09</v>
+      </c>
+      <c r="D6">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>8.1491679999999995</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="I6">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>0.15166666666666667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>12.09</v>
+      </c>
+      <c r="B7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="2"/>
+        <v>F17-18B-12.09</v>
+      </c>
+      <c r="D7">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1.5500610000000008</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>0.128</v>
+      </c>
+      <c r="I7">
+        <v>0.13</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>8.6000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>12.09</v>
+      </c>
+      <c r="B8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="2"/>
+        <v>F16-17B-12.09</v>
+      </c>
+      <c r="D8">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>3.4721310000000005</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I8">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>4.6000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>12.09</v>
+      </c>
+      <c r="B9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="2"/>
+        <v>F17-18A-12.09</v>
+      </c>
+      <c r="D9">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>2.7033030000000005</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="I9">
+        <v>3.9E-2</v>
+      </c>
+      <c r="J9">
+        <f>SUM(H9:I9)/2</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>12.09</v>
+      </c>
+      <c r="B10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="2"/>
+        <v>F18-19-12.09</v>
+      </c>
+      <c r="D10">
+        <v>0.09</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>2.8955100000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>12.09</v>
+      </c>
+      <c r="B11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="2"/>
+        <v>F19-20A-12.09</v>
+      </c>
+      <c r="D11">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.84530200000000066</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>12.09</v>
+      </c>
+      <c r="B12" t="s">
+        <v>183</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="2"/>
+        <v>F16-17A-12.09</v>
+      </c>
+      <c r="D12">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>7.8288230000000016</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>14.09</v>
+      </c>
+      <c r="B13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="2"/>
+        <v>FP1-14.09</v>
+      </c>
+      <c r="D13">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <f>(64.069*AVERAGE(D13:D13)-2.8707)*E13</f>
+        <v>153.04639200000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>184</v>
+      </c>
+      <c r="D14">
+        <v>0.126</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14:F37" si="3">(64.069*AVERAGE(D14:D14)-2.8707)*E14</f>
+        <v>20.807976000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="3"/>
+        <v>39.259848000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <v>0.19</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="3"/>
+        <v>37.209640000000007</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="3"/>
+        <v>34.390604000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="3"/>
+        <v>39.003572000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19">
+        <v>0.183</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="3"/>
+        <v>35.415708000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D20">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="3"/>
+        <v>-2.5131399999999982</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="3"/>
+        <v>985.62932000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="E22">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="3"/>
+        <v>817.76854000000014</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23">
+        <v>0.51</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="3"/>
+        <v>298.04489999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="E24">
+        <v>10</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="3"/>
+        <v>216.03658000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25">
+        <v>0.31</v>
+      </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="3"/>
+        <v>169.90690000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>186</v>
+      </c>
+      <c r="D26">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="3"/>
+        <v>-0.71920799999999829</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="E27">
+        <v>20</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="3"/>
+        <v>812.64302000000021</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28">
+        <v>0.629</v>
+      </c>
+      <c r="E28">
+        <v>20</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="3"/>
+        <v>748.57402000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="E29">
+        <v>10</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="3"/>
+        <v>488.32983000000007</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30">
+        <v>0.626</v>
+      </c>
+      <c r="E30">
+        <v>10</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="3"/>
+        <v>372.36493999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>125</v>
+      </c>
+      <c r="D31">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="E31">
+        <v>10</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="3"/>
+        <v>328.79802000000007</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C32" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D32">
+        <v>5.5E-2</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="3"/>
+        <v>0.65309500000000043</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="3"/>
+        <v>-0.56421600000000005</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="3"/>
+        <v>-0.62828499999999954</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C35" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="3"/>
+        <v>-0.50014699999999968</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C36" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D36">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="3"/>
+        <v>-0.43607799999999974</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C37" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D37">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="3"/>
+        <v>-0.69235399999999947</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
more no2 no3 general data added
</commit_message>
<xml_diff>
--- a/data/exp_raw/ssexp_data.xlsx
+++ b/data/exp_raw/ssexp_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vcantarella/Documents/FuhrbergerColumns/data/exp_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BBF40B-AB9E-A84B-A02E-54BDD392B269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9CE55B-1902-1A41-B0FC-625C86104041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="800" windowWidth="28040" windowHeight="16680" activeTab="3" xr2:uid="{82067E57-95C1-4A4D-B858-7597035F15DE}"/>
+    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16680" activeTab="6" xr2:uid="{82067E57-95C1-4A4D-B858-7597035F15DE}"/>
   </bookViews>
   <sheets>
     <sheet name="general_samples_p1" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,9 @@
     <sheet name="fe" sheetId="2" r:id="rId5"/>
     <sheet name="hs" sheetId="3" r:id="rId6"/>
     <sheet name="standard_curve_no2" sheetId="7" r:id="rId7"/>
+    <sheet name="fe_plate_1" sheetId="8" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
   </externalReferences>
   <calcPr calcId="191029"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="291">
   <si>
     <t>Sample</t>
   </si>
@@ -616,6 +616,309 @@
   </si>
   <si>
     <t>* vial broke + cleaned pump tubing</t>
+  </si>
+  <si>
+    <t>time_label</t>
+  </si>
+  <si>
+    <t>column</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>val2</t>
+  </si>
+  <si>
+    <t>fe2+ [micromol/L]</t>
+  </si>
+  <si>
+    <t>Value 3</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>P1F3</t>
+  </si>
+  <si>
+    <t>P2F3</t>
+  </si>
+  <si>
+    <t>P3F3</t>
+  </si>
+  <si>
+    <t>P4F3</t>
+  </si>
+  <si>
+    <t>P1T36</t>
+  </si>
+  <si>
+    <t>P1T37</t>
+  </si>
+  <si>
+    <t>P1T38</t>
+  </si>
+  <si>
+    <t>P1T39</t>
+  </si>
+  <si>
+    <t>P1T40</t>
+  </si>
+  <si>
+    <t>P1T41</t>
+  </si>
+  <si>
+    <t>P1T42</t>
+  </si>
+  <si>
+    <t>P1T43</t>
+  </si>
+  <si>
+    <t>P1T44</t>
+  </si>
+  <si>
+    <t>P1T45</t>
+  </si>
+  <si>
+    <t>P1T46</t>
+  </si>
+  <si>
+    <t>P1T47</t>
+  </si>
+  <si>
+    <t>P1T48</t>
+  </si>
+  <si>
+    <t>P1T49</t>
+  </si>
+  <si>
+    <t>P1T50</t>
+  </si>
+  <si>
+    <t>P1T51</t>
+  </si>
+  <si>
+    <t>P1T52</t>
+  </si>
+  <si>
+    <t>P1T53</t>
+  </si>
+  <si>
+    <t>P1T54</t>
+  </si>
+  <si>
+    <t>P1T55</t>
+  </si>
+  <si>
+    <t>P2T36</t>
+  </si>
+  <si>
+    <t>P2T37</t>
+  </si>
+  <si>
+    <t>P2T38</t>
+  </si>
+  <si>
+    <t>P2T39</t>
+  </si>
+  <si>
+    <t>P2T40</t>
+  </si>
+  <si>
+    <t>P2T41</t>
+  </si>
+  <si>
+    <t>P2T42</t>
+  </si>
+  <si>
+    <t>P2T43</t>
+  </si>
+  <si>
+    <t>P2T44</t>
+  </si>
+  <si>
+    <t>P2T45</t>
+  </si>
+  <si>
+    <t>P2T46</t>
+  </si>
+  <si>
+    <t>P2T47</t>
+  </si>
+  <si>
+    <t>P2T48</t>
+  </si>
+  <si>
+    <t>P2T49</t>
+  </si>
+  <si>
+    <t>P2T50</t>
+  </si>
+  <si>
+    <t>P2T51</t>
+  </si>
+  <si>
+    <t>P2T52</t>
+  </si>
+  <si>
+    <t>P2T53</t>
+  </si>
+  <si>
+    <t>P2T54</t>
+  </si>
+  <si>
+    <t>P2T55</t>
+  </si>
+  <si>
+    <t>P3T36</t>
+  </si>
+  <si>
+    <t>P3T37</t>
+  </si>
+  <si>
+    <t>P3T38</t>
+  </si>
+  <si>
+    <t>P3T39</t>
+  </si>
+  <si>
+    <t>P3T40</t>
+  </si>
+  <si>
+    <t>P3T41</t>
+  </si>
+  <si>
+    <t>P3T42</t>
+  </si>
+  <si>
+    <t>P3T43</t>
+  </si>
+  <si>
+    <t>P3T44</t>
+  </si>
+  <si>
+    <t>P3T45</t>
+  </si>
+  <si>
+    <t>P3T46</t>
+  </si>
+  <si>
+    <t>P3T47</t>
+  </si>
+  <si>
+    <t>P3T48</t>
+  </si>
+  <si>
+    <t>P3T49</t>
+  </si>
+  <si>
+    <t>P3T50</t>
+  </si>
+  <si>
+    <t>P3T51</t>
+  </si>
+  <si>
+    <t>P3T52</t>
+  </si>
+  <si>
+    <t>P3T53</t>
+  </si>
+  <si>
+    <t>P3T54</t>
+  </si>
+  <si>
+    <t>P3T55</t>
+  </si>
+  <si>
+    <t>P4T36</t>
+  </si>
+  <si>
+    <t>P4T37</t>
+  </si>
+  <si>
+    <t>P4T38</t>
+  </si>
+  <si>
+    <t>P4T39</t>
+  </si>
+  <si>
+    <t>P4T40</t>
+  </si>
+  <si>
+    <t>P4T41</t>
+  </si>
+  <si>
+    <t>P4T42</t>
+  </si>
+  <si>
+    <t>P4T43</t>
+  </si>
+  <si>
+    <t>P4T44</t>
+  </si>
+  <si>
+    <t>P4T45</t>
+  </si>
+  <si>
+    <t>P4T46</t>
+  </si>
+  <si>
+    <t>P4T47</t>
+  </si>
+  <si>
+    <t>P4T48</t>
+  </si>
+  <si>
+    <t>P4T49</t>
+  </si>
+  <si>
+    <t>P4T50</t>
+  </si>
+  <si>
+    <t>P4T51</t>
+  </si>
+  <si>
+    <t>P4T52</t>
+  </si>
+  <si>
+    <t>P4T53</t>
+  </si>
+  <si>
+    <t>P4T54</t>
+  </si>
+  <si>
+    <t>P4T55</t>
+  </si>
+  <si>
+    <t>P1T56</t>
+  </si>
+  <si>
+    <t>P1T57</t>
+  </si>
+  <si>
+    <t>P1T58</t>
+  </si>
+  <si>
+    <t>P1T59</t>
+  </si>
+  <si>
+    <t>P1T60</t>
+  </si>
+  <si>
+    <t>P1T61</t>
+  </si>
+  <si>
+    <t>P1T62</t>
+  </si>
+  <si>
+    <t>P1T63</t>
+  </si>
+  <si>
+    <t>* auto smapler failed</t>
+  </si>
+  <si>
+    <t>* vial leaked (bad cap)</t>
   </si>
 </sst>
 </file>
@@ -905,7 +1208,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'[2]standard_curve_plate 2'!$H$2:$H$8</c:f>
+              <c:f>'[1]standard_curve_plate 2'!$H$2:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1097,6 +1400,421 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fe_plate_1!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.40496723804367729"/>
+                  <c:y val="-3.6085010650264461E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-DE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>fe_plate_1!$M$3:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.82450000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.42599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1915</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.7499999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5999999999999994E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>fe_plate_1!$I$3:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-965F-5541-BCF4-A4E25A2584BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="683948543"/>
+        <c:axId val="683950255"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="683948543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="683950255"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="683950255"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="683948543"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1137,7 +1855,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1696,66 +2970,50 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="standard_curve_no2-test"/>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="J2">
-            <v>0.59166666666666667</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="J3">
-            <v>0.48500000000000004</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="J4">
-            <v>0.34966666666666663</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="J5">
-            <v>0.27066666666666667</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="J6">
-            <v>0.15166666666666667</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="J7">
-            <v>8.6000000000000007E-2</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="J8">
-            <v>4.6000000000000006E-2</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="J9">
-            <v>4.4999999999999998E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA1D0600-A7AC-0A46-ABE2-1798D8ACE7F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -2144,10 +3402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE2E69C-B565-9948-8744-019B7DBC9C60}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2210,7 +3468,7 @@
         <v>18.91</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E28" si="0">(D2-6.75)/6</f>
+        <f t="shared" ref="E2:E48" si="0">(D2-6.75)/6</f>
         <v>2.0266666666666668</v>
       </c>
     </row>
@@ -2786,6 +4044,13 @@
         <f t="shared" si="2"/>
         <v>45929.71597222222</v>
       </c>
+      <c r="D29">
+        <v>20.87</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>2.3533333333333335</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -2799,6 +4064,13 @@
         <f t="shared" si="2"/>
         <v>45929.96597222222</v>
       </c>
+      <c r="D30">
+        <v>20.440000000000001</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>2.2816666666666667</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -2812,6 +4084,13 @@
         <f t="shared" si="2"/>
         <v>45930.21597222222</v>
       </c>
+      <c r="D31">
+        <v>19.420000000000002</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>2.1116666666666668</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -2825,8 +4104,15 @@
         <f t="shared" si="2"/>
         <v>45930.46597222222</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>19.97</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>2.2033333333333331</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -2839,7 +4125,7 @@
         <v>45930.71597222222</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -2851,8 +4137,15 @@
         <f t="shared" si="2"/>
         <v>45930.96597222222</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>19.61</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>2.1433333333333331</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>78</v>
       </c>
@@ -2864,8 +4157,15 @@
         <f t="shared" si="2"/>
         <v>45931.21597222222</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>19.5</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>2.125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -2876,6 +4176,491 @@
       <c r="C36" s="1">
         <f t="shared" si="2"/>
         <v>45931.46597222222</v>
+      </c>
+      <c r="D36">
+        <v>19.39</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>2.1066666666666669</v>
+      </c>
+      <c r="F36">
+        <v>8.14</v>
+      </c>
+      <c r="G36">
+        <v>897</v>
+      </c>
+      <c r="H36">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>201</v>
+      </c>
+      <c r="B37" s="1">
+        <f t="shared" ref="B37:B49" si="3">C36</f>
+        <v>45931.46597222222</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" ref="C37:C49" si="4">B37+6/24</f>
+        <v>45931.71597222222</v>
+      </c>
+      <c r="D37">
+        <v>18.690000000000001</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>1.9900000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>202</v>
+      </c>
+      <c r="B38" s="1">
+        <f t="shared" si="3"/>
+        <v>45931.71597222222</v>
+      </c>
+      <c r="C38" s="1">
+        <f t="shared" si="4"/>
+        <v>45931.96597222222</v>
+      </c>
+      <c r="D38">
+        <v>18.61</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>1.9766666666666666</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>203</v>
+      </c>
+      <c r="B39" s="1">
+        <f t="shared" si="3"/>
+        <v>45931.96597222222</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" si="4"/>
+        <v>45932.21597222222</v>
+      </c>
+      <c r="D39">
+        <v>18.55</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>1.9666666666666668</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>204</v>
+      </c>
+      <c r="B40" s="1">
+        <f t="shared" si="3"/>
+        <v>45932.21597222222</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" si="4"/>
+        <v>45932.46597222222</v>
+      </c>
+      <c r="D40">
+        <v>18.52</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>1.9616666666666667</v>
+      </c>
+      <c r="F40">
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="G40">
+        <v>866</v>
+      </c>
+      <c r="H40">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>205</v>
+      </c>
+      <c r="B41" s="1">
+        <f t="shared" si="3"/>
+        <v>45932.46597222222</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" si="4"/>
+        <v>45932.71597222222</v>
+      </c>
+      <c r="D41">
+        <v>18.54</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>1.9649999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>206</v>
+      </c>
+      <c r="B42" s="1">
+        <f t="shared" si="3"/>
+        <v>45932.71597222222</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" si="4"/>
+        <v>45932.96597222222</v>
+      </c>
+      <c r="D42">
+        <v>18.28</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>1.9216666666666669</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>207</v>
+      </c>
+      <c r="B43" s="1">
+        <f t="shared" si="3"/>
+        <v>45932.96597222222</v>
+      </c>
+      <c r="C43" s="1">
+        <f t="shared" si="4"/>
+        <v>45933.21597222222</v>
+      </c>
+      <c r="D43">
+        <v>18.28</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>1.9216666666666669</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>208</v>
+      </c>
+      <c r="B44" s="1">
+        <f t="shared" si="3"/>
+        <v>45933.21597222222</v>
+      </c>
+      <c r="C44" s="1">
+        <f t="shared" si="4"/>
+        <v>45933.46597222222</v>
+      </c>
+      <c r="D44">
+        <v>18.3</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>1.925</v>
+      </c>
+      <c r="H44">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>209</v>
+      </c>
+      <c r="B45" s="1">
+        <f t="shared" si="3"/>
+        <v>45933.46597222222</v>
+      </c>
+      <c r="C45" s="1">
+        <f t="shared" si="4"/>
+        <v>45933.71597222222</v>
+      </c>
+      <c r="D45">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>1.9299999999999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>210</v>
+      </c>
+      <c r="B46" s="1">
+        <f t="shared" si="3"/>
+        <v>45933.71597222222</v>
+      </c>
+      <c r="C46" s="1">
+        <f t="shared" si="4"/>
+        <v>45933.96597222222</v>
+      </c>
+      <c r="D46">
+        <v>17.13</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>1.7299999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>211</v>
+      </c>
+      <c r="B47" s="1">
+        <f t="shared" si="3"/>
+        <v>45933.96597222222</v>
+      </c>
+      <c r="C47" s="1">
+        <f t="shared" si="4"/>
+        <v>45934.21597222222</v>
+      </c>
+      <c r="D47">
+        <v>18.28</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>1.9216666666666669</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>212</v>
+      </c>
+      <c r="B48" s="1">
+        <f t="shared" si="3"/>
+        <v>45934.21597222222</v>
+      </c>
+      <c r="C48" s="1">
+        <f t="shared" si="4"/>
+        <v>45934.46597222222</v>
+      </c>
+      <c r="D48">
+        <v>18.309999999999999</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>1.9266666666666665</v>
+      </c>
+      <c r="F48">
+        <v>8.32</v>
+      </c>
+      <c r="G48">
+        <v>855</v>
+      </c>
+      <c r="H48">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>213</v>
+      </c>
+      <c r="B49" s="1">
+        <f t="shared" si="3"/>
+        <v>45934.46597222222</v>
+      </c>
+      <c r="C49" s="1">
+        <f t="shared" si="4"/>
+        <v>45934.71597222222</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>214</v>
+      </c>
+      <c r="B50" s="1">
+        <f t="shared" ref="B50:B56" si="5">C49</f>
+        <v>45934.71597222222</v>
+      </c>
+      <c r="C50" s="1">
+        <f t="shared" ref="C50:C56" si="6">B50+6/24</f>
+        <v>45934.96597222222</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>215</v>
+      </c>
+      <c r="B51" s="1">
+        <f t="shared" si="5"/>
+        <v>45934.96597222222</v>
+      </c>
+      <c r="C51" s="1">
+        <f t="shared" si="6"/>
+        <v>45935.21597222222</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>216</v>
+      </c>
+      <c r="B52" s="1">
+        <f t="shared" si="5"/>
+        <v>45935.21597222222</v>
+      </c>
+      <c r="C52" s="1">
+        <f t="shared" si="6"/>
+        <v>45935.46597222222</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>217</v>
+      </c>
+      <c r="B53" s="1">
+        <f t="shared" si="5"/>
+        <v>45935.46597222222</v>
+      </c>
+      <c r="C53" s="1">
+        <f t="shared" si="6"/>
+        <v>45935.71597222222</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>218</v>
+      </c>
+      <c r="B54" s="1">
+        <f t="shared" si="5"/>
+        <v>45935.71597222222</v>
+      </c>
+      <c r="C54" s="1">
+        <f t="shared" si="6"/>
+        <v>45935.96597222222</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>219</v>
+      </c>
+      <c r="B55" s="1">
+        <f t="shared" si="5"/>
+        <v>45935.96597222222</v>
+      </c>
+      <c r="C55" s="1">
+        <f t="shared" si="6"/>
+        <v>45936.21597222222</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>220</v>
+      </c>
+      <c r="B56" s="1">
+        <f t="shared" si="5"/>
+        <v>45936.21597222222</v>
+      </c>
+      <c r="C56" s="1">
+        <f t="shared" si="6"/>
+        <v>45936.46597222222</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>281</v>
+      </c>
+      <c r="B57" s="1">
+        <f t="shared" ref="B57:B64" si="7">C56</f>
+        <v>45936.46597222222</v>
+      </c>
+      <c r="C57" s="1">
+        <f t="shared" ref="C57:C64" si="8">B57+6/24</f>
+        <v>45936.71597222222</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>282</v>
+      </c>
+      <c r="B58" s="1">
+        <f t="shared" si="7"/>
+        <v>45936.71597222222</v>
+      </c>
+      <c r="C58" s="1">
+        <f t="shared" si="8"/>
+        <v>45936.96597222222</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>283</v>
+      </c>
+      <c r="B59" s="1">
+        <f t="shared" si="7"/>
+        <v>45936.96597222222</v>
+      </c>
+      <c r="C59" s="1">
+        <f t="shared" si="8"/>
+        <v>45937.21597222222</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>284</v>
+      </c>
+      <c r="B60" s="1">
+        <f t="shared" si="7"/>
+        <v>45937.21597222222</v>
+      </c>
+      <c r="C60" s="1">
+        <f t="shared" si="8"/>
+        <v>45937.46597222222</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>285</v>
+      </c>
+      <c r="B61" s="1">
+        <f t="shared" si="7"/>
+        <v>45937.46597222222</v>
+      </c>
+      <c r="C61" s="1">
+        <f t="shared" si="8"/>
+        <v>45937.71597222222</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>286</v>
+      </c>
+      <c r="B62" s="1">
+        <f t="shared" si="7"/>
+        <v>45937.71597222222</v>
+      </c>
+      <c r="C62" s="1">
+        <f t="shared" si="8"/>
+        <v>45937.96597222222</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>287</v>
+      </c>
+      <c r="B63" s="1">
+        <f t="shared" si="7"/>
+        <v>45937.96597222222</v>
+      </c>
+      <c r="C63" s="1">
+        <f t="shared" si="8"/>
+        <v>45938.21597222222</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>288</v>
+      </c>
+      <c r="B64" s="1">
+        <f t="shared" si="7"/>
+        <v>45938.21597222222</v>
+      </c>
+      <c r="C64" s="1">
+        <f t="shared" si="8"/>
+        <v>45938.46597222222</v>
       </c>
     </row>
   </sheetData>
@@ -2888,8 +4673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046BB4A8-8683-FF42-8F76-0A791D85765F}">
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2950,7 +4735,7 @@
         <v>17.7</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E27" si="0">(D2-6.75)/6</f>
+        <f t="shared" ref="E2:E26" si="0">(D2-6.75)/6</f>
         <v>1.825</v>
       </c>
     </row>
@@ -3478,7 +5263,7 @@
         <v>19.63</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
+        <f>(D27-6.75)/6</f>
         <v>2.1466666666666665</v>
       </c>
       <c r="F27">
@@ -3519,6 +5304,13 @@
         <f t="shared" si="2"/>
         <v>45929.71597222222</v>
       </c>
+      <c r="D29">
+        <v>22.34</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ref="E29:E46" si="3">(D29-6.75)/6</f>
+        <v>2.5983333333333332</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -3532,6 +5324,13 @@
         <f t="shared" si="2"/>
         <v>45929.96597222222</v>
       </c>
+      <c r="D30">
+        <v>21.75</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="3"/>
+        <v>2.5</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -3545,6 +5344,13 @@
         <f t="shared" si="2"/>
         <v>45930.21597222222</v>
       </c>
+      <c r="D31">
+        <v>21.34</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="3"/>
+        <v>2.4316666666666666</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -3558,8 +5364,15 @@
         <f t="shared" si="2"/>
         <v>45930.46597222222</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>20.98</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="3"/>
+        <v>2.3716666666666666</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>103</v>
       </c>
@@ -3572,7 +5385,7 @@
         <v>45930.71597222222</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -3584,8 +5397,15 @@
         <f t="shared" si="2"/>
         <v>45930.96597222222</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>18.440000000000001</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="3"/>
+        <v>1.9483333333333335</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>105</v>
       </c>
@@ -3597,8 +5417,15 @@
         <f t="shared" si="2"/>
         <v>45931.21597222222</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>18.43</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="3"/>
+        <v>1.9466666666666665</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>106</v>
       </c>
@@ -3610,108 +5437,398 @@
         <f t="shared" si="2"/>
         <v>45931.46597222222</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <v>18.27</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="3"/>
+        <v>1.92</v>
+      </c>
+      <c r="F36">
+        <v>7.95</v>
+      </c>
+      <c r="G36">
+        <v>765</v>
+      </c>
+      <c r="H36">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>221</v>
+      </c>
+      <c r="B37" s="1">
+        <f t="shared" ref="B37:B56" si="4">C36</f>
+        <v>45931.46597222222</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" ref="C37:C56" si="5">B37+6/24</f>
+        <v>45931.71597222222</v>
+      </c>
+      <c r="D37">
+        <v>18.89</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="3"/>
+        <v>2.0233333333333334</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>222</v>
+      </c>
+      <c r="B38" s="1">
+        <f t="shared" si="4"/>
+        <v>45931.71597222222</v>
+      </c>
+      <c r="C38" s="1">
+        <f t="shared" si="5"/>
+        <v>45931.96597222222</v>
+      </c>
+      <c r="D38">
+        <v>18.7</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="3"/>
+        <v>1.9916666666666665</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>223</v>
+      </c>
+      <c r="B39" s="1">
+        <f t="shared" si="4"/>
+        <v>45931.96597222222</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" si="5"/>
+        <v>45932.21597222222</v>
+      </c>
+      <c r="D39">
+        <v>18.649999999999999</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="3"/>
+        <v>1.9833333333333332</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>224</v>
+      </c>
+      <c r="B40" s="1">
+        <f t="shared" si="4"/>
+        <v>45932.21597222222</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" si="5"/>
+        <v>45932.46597222222</v>
+      </c>
+      <c r="D40">
+        <v>18.64</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="3"/>
+        <v>1.9816666666666667</v>
+      </c>
+      <c r="F40">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="G40">
+        <v>867</v>
+      </c>
+      <c r="H40">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>225</v>
+      </c>
+      <c r="B41" s="1">
+        <f t="shared" si="4"/>
+        <v>45932.46597222222</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" si="5"/>
+        <v>45932.71597222222</v>
+      </c>
+      <c r="D41">
+        <v>18.54</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="3"/>
+        <v>1.9649999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>226</v>
+      </c>
+      <c r="B42" s="1">
+        <f t="shared" si="4"/>
+        <v>45932.71597222222</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" si="5"/>
+        <v>45932.96597222222</v>
+      </c>
+      <c r="D42">
+        <v>18.89</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="3"/>
+        <v>2.0233333333333334</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>227</v>
+      </c>
+      <c r="B43" s="1">
+        <f t="shared" si="4"/>
+        <v>45932.96597222222</v>
+      </c>
+      <c r="C43" s="1">
+        <f t="shared" si="5"/>
+        <v>45933.21597222222</v>
+      </c>
+      <c r="D43">
+        <v>18.989999999999998</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="3"/>
+        <v>2.0399999999999996</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>228</v>
+      </c>
+      <c r="B44" s="1">
+        <f t="shared" si="4"/>
+        <v>45933.21597222222</v>
+      </c>
+      <c r="C44" s="1">
+        <f t="shared" si="5"/>
+        <v>45933.46597222222</v>
+      </c>
+      <c r="D44">
+        <v>19.010000000000002</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="3"/>
+        <v>2.0433333333333334</v>
+      </c>
+      <c r="H44">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>229</v>
+      </c>
+      <c r="B45" s="1">
+        <f t="shared" si="4"/>
+        <v>45933.46597222222</v>
+      </c>
+      <c r="C45" s="1">
+        <f t="shared" si="5"/>
+        <v>45933.71597222222</v>
+      </c>
+      <c r="D45">
+        <v>19.010000000000002</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="3"/>
+        <v>2.0433333333333334</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>230</v>
+      </c>
+      <c r="B46" s="1">
+        <f t="shared" si="4"/>
+        <v>45933.71597222222</v>
+      </c>
+      <c r="C46" s="1">
+        <f t="shared" si="5"/>
+        <v>45933.96597222222</v>
+      </c>
+      <c r="D46">
+        <v>18.96</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="3"/>
+        <v>2.0350000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>231</v>
+      </c>
+      <c r="B47" s="1">
+        <f t="shared" si="4"/>
+        <v>45933.96597222222</v>
+      </c>
+      <c r="C47" s="1">
+        <f t="shared" si="5"/>
+        <v>45934.21597222222</v>
+      </c>
+      <c r="F47">
+        <v>8.18</v>
+      </c>
+      <c r="G47">
+        <v>853</v>
+      </c>
+      <c r="H47">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>232</v>
+      </c>
+      <c r="B48" s="1">
+        <f t="shared" si="4"/>
+        <v>45934.21597222222</v>
+      </c>
+      <c r="C48" s="1">
+        <f t="shared" si="5"/>
+        <v>45934.46597222222</v>
+      </c>
+      <c r="L48" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>233</v>
+      </c>
+      <c r="B49" s="1">
+        <f t="shared" si="4"/>
+        <v>45934.46597222222</v>
+      </c>
+      <c r="C49" s="1">
+        <f t="shared" si="5"/>
+        <v>45934.71597222222</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>234</v>
+      </c>
+      <c r="B50" s="1">
+        <f t="shared" si="4"/>
+        <v>45934.71597222222</v>
+      </c>
+      <c r="C50" s="1">
+        <f t="shared" si="5"/>
+        <v>45934.96597222222</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>235</v>
+      </c>
+      <c r="B51" s="1">
+        <f t="shared" si="4"/>
+        <v>45934.96597222222</v>
+      </c>
+      <c r="C51" s="1">
+        <f t="shared" si="5"/>
+        <v>45935.21597222222</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>236</v>
+      </c>
+      <c r="B52" s="1">
+        <f t="shared" si="4"/>
+        <v>45935.21597222222</v>
+      </c>
+      <c r="C52" s="1">
+        <f t="shared" si="5"/>
+        <v>45935.46597222222</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>237</v>
+      </c>
+      <c r="B53" s="1">
+        <f t="shared" si="4"/>
+        <v>45935.46597222222</v>
+      </c>
+      <c r="C53" s="1">
+        <f t="shared" si="5"/>
+        <v>45935.71597222222</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>238</v>
+      </c>
+      <c r="B54" s="1">
+        <f t="shared" si="4"/>
+        <v>45935.71597222222</v>
+      </c>
+      <c r="C54" s="1">
+        <f t="shared" si="5"/>
+        <v>45935.96597222222</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>239</v>
+      </c>
+      <c r="B55" s="1">
+        <f t="shared" si="4"/>
+        <v>45935.96597222222</v>
+      </c>
+      <c r="C55" s="1">
+        <f t="shared" si="5"/>
+        <v>45936.21597222222</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>240</v>
+      </c>
+      <c r="B56" s="1">
+        <f t="shared" si="4"/>
+        <v>45936.21597222222</v>
+      </c>
+      <c r="C56" s="1">
+        <f t="shared" si="5"/>
+        <v>45936.46597222222</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
     </row>
@@ -3723,10 +5840,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{649DD004-07E5-F04F-B76F-816E14D1C8AC}">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3787,7 +5904,7 @@
         <v>17.64</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E28" si="0">(D2-6.75)/6</f>
+        <f t="shared" ref="E2:E48" si="0">(D2-6.75)/6</f>
         <v>1.8150000000000002</v>
       </c>
     </row>
@@ -4363,6 +6480,13 @@
         <f t="shared" si="2"/>
         <v>45929.71597222222</v>
       </c>
+      <c r="D29">
+        <v>22.55</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>2.6333333333333333</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -4376,6 +6500,13 @@
         <f t="shared" si="2"/>
         <v>45929.96597222222</v>
       </c>
+      <c r="D30">
+        <v>22.41</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>2.61</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -4389,6 +6520,13 @@
         <f t="shared" si="2"/>
         <v>45930.21597222222</v>
       </c>
+      <c r="D31">
+        <v>22.18</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>2.5716666666666668</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -4402,8 +6540,15 @@
         <f t="shared" si="2"/>
         <v>45930.46597222222</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>21.67</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>2.4866666666666668</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>130</v>
       </c>
@@ -4416,7 +6561,7 @@
         <v>45930.71597222222</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>131</v>
       </c>
@@ -4428,8 +6573,15 @@
         <f t="shared" si="2"/>
         <v>45930.96597222222</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>19.86</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>2.1850000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>132</v>
       </c>
@@ -4441,8 +6593,15 @@
         <f t="shared" si="2"/>
         <v>45931.21597222222</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>20.260000000000002</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>2.2516666666666669</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>133</v>
       </c>
@@ -4454,66 +6613,383 @@
         <f t="shared" si="2"/>
         <v>45931.46597222222</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
+      <c r="D36">
+        <v>19.84</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>2.1816666666666666</v>
+      </c>
+      <c r="F36">
+        <v>7.96</v>
+      </c>
+      <c r="G36">
+        <v>831</v>
+      </c>
+      <c r="H36">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>241</v>
+      </c>
+      <c r="B37" s="1">
+        <f t="shared" ref="B37:B55" si="3">C36</f>
+        <v>45931.46597222222</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" ref="C37:C55" si="4">B37+6/24</f>
+        <v>45931.71597222222</v>
+      </c>
+      <c r="D37">
+        <v>19.64</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>2.1483333333333334</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>242</v>
+      </c>
+      <c r="B38" s="1">
+        <f t="shared" si="3"/>
+        <v>45931.71597222222</v>
+      </c>
+      <c r="C38" s="1">
+        <f t="shared" si="4"/>
+        <v>45931.96597222222</v>
+      </c>
+      <c r="D38">
+        <v>19.37</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>2.1033333333333335</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>243</v>
+      </c>
+      <c r="B39" s="1">
+        <f t="shared" si="3"/>
+        <v>45931.96597222222</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" si="4"/>
+        <v>45932.21597222222</v>
+      </c>
+      <c r="D39">
+        <v>19.05</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>2.0500000000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>244</v>
+      </c>
+      <c r="B40" s="1">
+        <f t="shared" si="3"/>
+        <v>45932.21597222222</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" si="4"/>
+        <v>45932.46597222222</v>
+      </c>
+      <c r="D40">
+        <v>19.28</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>2.0883333333333334</v>
+      </c>
+      <c r="F40">
+        <v>8.06</v>
+      </c>
+      <c r="G40">
+        <v>876</v>
+      </c>
+      <c r="H40">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>245</v>
+      </c>
+      <c r="B41" s="1">
+        <f t="shared" si="3"/>
+        <v>45932.46597222222</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" si="4"/>
+        <v>45932.71597222222</v>
+      </c>
+      <c r="D41">
+        <v>19.05</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>2.0500000000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>246</v>
+      </c>
+      <c r="B42" s="1">
+        <f t="shared" si="3"/>
+        <v>45932.71597222222</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" si="4"/>
+        <v>45932.96597222222</v>
+      </c>
+      <c r="D42">
+        <v>18.97</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>2.0366666666666666</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>247</v>
+      </c>
+      <c r="B43" s="1">
+        <f t="shared" si="3"/>
+        <v>45932.96597222222</v>
+      </c>
+      <c r="C43" s="1">
+        <f t="shared" si="4"/>
+        <v>45933.21597222222</v>
+      </c>
+      <c r="D43">
+        <v>19.04</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>2.0483333333333333</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>248</v>
+      </c>
+      <c r="B44" s="1">
+        <f t="shared" si="3"/>
+        <v>45933.21597222222</v>
+      </c>
+      <c r="C44" s="1">
+        <f t="shared" si="4"/>
+        <v>45933.46597222222</v>
+      </c>
+      <c r="D44">
+        <v>18.97</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>2.0366666666666666</v>
+      </c>
+      <c r="H44">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>249</v>
+      </c>
+      <c r="B45" s="1">
+        <f t="shared" si="3"/>
+        <v>45933.46597222222</v>
+      </c>
+      <c r="C45" s="1">
+        <f t="shared" si="4"/>
+        <v>45933.71597222222</v>
+      </c>
+      <c r="D45">
+        <v>19.02</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>2.0449999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>250</v>
+      </c>
+      <c r="B46" s="1">
+        <f t="shared" si="3"/>
+        <v>45933.71597222222</v>
+      </c>
+      <c r="C46" s="1">
+        <f t="shared" si="4"/>
+        <v>45933.96597222222</v>
+      </c>
+      <c r="L46" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>251</v>
+      </c>
+      <c r="B47" s="1">
+        <f t="shared" si="3"/>
+        <v>45933.96597222222</v>
+      </c>
+      <c r="C47" s="1">
+        <f t="shared" si="4"/>
+        <v>45934.21597222222</v>
+      </c>
+      <c r="D47">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>2.0249999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>252</v>
+      </c>
+      <c r="B48" s="1">
+        <f t="shared" si="3"/>
+        <v>45934.21597222222</v>
+      </c>
+      <c r="C48" s="1">
+        <f t="shared" si="4"/>
+        <v>45934.46597222222</v>
+      </c>
+      <c r="D48">
+        <v>18.98</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>2.0383333333333336</v>
+      </c>
+      <c r="F48">
+        <v>8.35</v>
+      </c>
+      <c r="G48">
+        <v>862</v>
+      </c>
+      <c r="H48">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>253</v>
+      </c>
+      <c r="B49" s="1">
+        <f t="shared" si="3"/>
+        <v>45934.46597222222</v>
+      </c>
+      <c r="C49" s="1">
+        <f t="shared" si="4"/>
+        <v>45934.71597222222</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>254</v>
+      </c>
+      <c r="B50" s="1">
+        <f t="shared" si="3"/>
+        <v>45934.71597222222</v>
+      </c>
+      <c r="C50" s="1">
+        <f t="shared" si="4"/>
+        <v>45934.96597222222</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>255</v>
+      </c>
+      <c r="B51" s="1">
+        <f t="shared" si="3"/>
+        <v>45934.96597222222</v>
+      </c>
+      <c r="C51" s="1">
+        <f t="shared" si="4"/>
+        <v>45935.21597222222</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>256</v>
+      </c>
+      <c r="B52" s="1">
+        <f t="shared" si="3"/>
+        <v>45935.21597222222</v>
+      </c>
+      <c r="C52" s="1">
+        <f t="shared" si="4"/>
+        <v>45935.46597222222</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>257</v>
+      </c>
+      <c r="B53" s="1">
+        <f t="shared" si="3"/>
+        <v>45935.46597222222</v>
+      </c>
+      <c r="C53" s="1">
+        <f t="shared" si="4"/>
+        <v>45935.71597222222</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>258</v>
+      </c>
+      <c r="B54" s="1">
+        <f t="shared" si="3"/>
+        <v>45935.71597222222</v>
+      </c>
+      <c r="C54" s="1">
+        <f t="shared" si="4"/>
+        <v>45935.96597222222</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>259</v>
+      </c>
+      <c r="B55" s="1">
+        <f t="shared" si="3"/>
+        <v>45935.96597222222</v>
+      </c>
+      <c r="C55" s="1">
+        <f t="shared" si="4"/>
+        <v>45936.21597222222</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>260</v>
+      </c>
+      <c r="B56" s="1">
+        <f t="shared" ref="B56" si="5">C55</f>
+        <v>45936.21597222222</v>
+      </c>
+      <c r="C56" s="1">
+        <f t="shared" ref="C56" si="6">B56+6/24</f>
+        <v>45936.46597222222</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4523,10 +6999,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CEAE0A4-BA85-AC4B-952F-A9D4082FC119}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4587,7 +7063,7 @@
         <v>18.05</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E28" si="0">(D2-6.75)/6</f>
+        <f t="shared" ref="E2:E48" si="0">(D2-6.75)/6</f>
         <v>1.8833333333333335</v>
       </c>
     </row>
@@ -5163,6 +7639,13 @@
         <f t="shared" si="2"/>
         <v>45929.71597222222</v>
       </c>
+      <c r="D29">
+        <v>22.73</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>2.6633333333333336</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -5176,6 +7659,13 @@
         <f t="shared" si="2"/>
         <v>45929.96597222222</v>
       </c>
+      <c r="D30">
+        <v>23.03</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>2.7133333333333334</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -5189,6 +7679,13 @@
         <f t="shared" si="2"/>
         <v>45930.21597222222</v>
       </c>
+      <c r="D31">
+        <v>23.19</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>2.74</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -5202,8 +7699,15 @@
         <f t="shared" si="2"/>
         <v>45930.46597222222</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>23.2</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>2.7416666666666667</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>157</v>
       </c>
@@ -5216,7 +7720,7 @@
         <v>45930.71597222222</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>158</v>
       </c>
@@ -5228,8 +7732,15 @@
         <f t="shared" si="2"/>
         <v>45930.96597222222</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>21.38</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>2.438333333333333</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>159</v>
       </c>
@@ -5241,8 +7752,15 @@
         <f t="shared" si="2"/>
         <v>45931.21597222222</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>21.15</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>160</v>
       </c>
@@ -5253,6 +7771,375 @@
       <c r="C36" s="1">
         <f t="shared" si="2"/>
         <v>45931.46597222222</v>
+      </c>
+      <c r="D36">
+        <v>21.08</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>2.3883333333333332</v>
+      </c>
+      <c r="F36">
+        <v>7.86</v>
+      </c>
+      <c r="G36">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>261</v>
+      </c>
+      <c r="B37" s="1">
+        <f t="shared" ref="B37:B56" si="3">C36</f>
+        <v>45931.46597222222</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" ref="C37:C56" si="4">B37+6/24</f>
+        <v>45931.71597222222</v>
+      </c>
+      <c r="D37">
+        <v>18.920000000000002</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>2.0283333333333338</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>262</v>
+      </c>
+      <c r="B38" s="1">
+        <f t="shared" si="3"/>
+        <v>45931.71597222222</v>
+      </c>
+      <c r="C38" s="1">
+        <f t="shared" si="4"/>
+        <v>45931.96597222222</v>
+      </c>
+      <c r="D38">
+        <v>18.940000000000001</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>2.0316666666666667</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>263</v>
+      </c>
+      <c r="B39" s="1">
+        <f t="shared" si="3"/>
+        <v>45931.96597222222</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" si="4"/>
+        <v>45932.21597222222</v>
+      </c>
+      <c r="D39">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>1.9299999999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>264</v>
+      </c>
+      <c r="B40" s="1">
+        <f t="shared" si="3"/>
+        <v>45932.21597222222</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" si="4"/>
+        <v>45932.46597222222</v>
+      </c>
+      <c r="D40">
+        <v>18.63</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>1.9799999999999998</v>
+      </c>
+      <c r="F40">
+        <v>7.88</v>
+      </c>
+      <c r="G40">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>265</v>
+      </c>
+      <c r="B41" s="1">
+        <f t="shared" si="3"/>
+        <v>45932.46597222222</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" si="4"/>
+        <v>45932.71597222222</v>
+      </c>
+      <c r="D41">
+        <v>18.63</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>1.9799999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>266</v>
+      </c>
+      <c r="B42" s="1">
+        <f t="shared" si="3"/>
+        <v>45932.71597222222</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" si="4"/>
+        <v>45932.96597222222</v>
+      </c>
+      <c r="D42">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>1.9299999999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>267</v>
+      </c>
+      <c r="B43" s="1">
+        <f t="shared" si="3"/>
+        <v>45932.96597222222</v>
+      </c>
+      <c r="C43" s="1">
+        <f t="shared" si="4"/>
+        <v>45933.21597222222</v>
+      </c>
+      <c r="D43">
+        <v>18.27</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>268</v>
+      </c>
+      <c r="B44" s="1">
+        <f t="shared" si="3"/>
+        <v>45933.21597222222</v>
+      </c>
+      <c r="C44" s="1">
+        <f t="shared" si="4"/>
+        <v>45933.46597222222</v>
+      </c>
+      <c r="D44">
+        <v>18.28</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>1.9216666666666669</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>269</v>
+      </c>
+      <c r="B45" s="1">
+        <f t="shared" si="3"/>
+        <v>45933.46597222222</v>
+      </c>
+      <c r="C45" s="1">
+        <f t="shared" si="4"/>
+        <v>45933.71597222222</v>
+      </c>
+      <c r="D45">
+        <v>18.29</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>1.9233333333333331</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>270</v>
+      </c>
+      <c r="B46" s="1">
+        <f t="shared" si="3"/>
+        <v>45933.71597222222</v>
+      </c>
+      <c r="C46" s="1">
+        <f t="shared" si="4"/>
+        <v>45933.96597222222</v>
+      </c>
+      <c r="D46">
+        <v>18.309999999999999</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>1.9266666666666665</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>271</v>
+      </c>
+      <c r="B47" s="1">
+        <f t="shared" si="3"/>
+        <v>45933.96597222222</v>
+      </c>
+      <c r="C47" s="1">
+        <f t="shared" si="4"/>
+        <v>45934.21597222222</v>
+      </c>
+      <c r="D47">
+        <v>18.29</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>1.9233333333333331</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>272</v>
+      </c>
+      <c r="B48" s="1">
+        <f t="shared" si="3"/>
+        <v>45934.21597222222</v>
+      </c>
+      <c r="C48" s="1">
+        <f t="shared" si="4"/>
+        <v>45934.46597222222</v>
+      </c>
+      <c r="D48">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>1.9299999999999997</v>
+      </c>
+      <c r="F48">
+        <v>8.16</v>
+      </c>
+      <c r="G48">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>273</v>
+      </c>
+      <c r="B49" s="1">
+        <f t="shared" si="3"/>
+        <v>45934.46597222222</v>
+      </c>
+      <c r="C49" s="1">
+        <f t="shared" si="4"/>
+        <v>45934.71597222222</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>274</v>
+      </c>
+      <c r="B50" s="1">
+        <f t="shared" si="3"/>
+        <v>45934.71597222222</v>
+      </c>
+      <c r="C50" s="1">
+        <f t="shared" si="4"/>
+        <v>45934.96597222222</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>275</v>
+      </c>
+      <c r="B51" s="1">
+        <f t="shared" si="3"/>
+        <v>45934.96597222222</v>
+      </c>
+      <c r="C51" s="1">
+        <f t="shared" si="4"/>
+        <v>45935.21597222222</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>276</v>
+      </c>
+      <c r="B52" s="1">
+        <f t="shared" si="3"/>
+        <v>45935.21597222222</v>
+      </c>
+      <c r="C52" s="1">
+        <f t="shared" si="4"/>
+        <v>45935.46597222222</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>277</v>
+      </c>
+      <c r="B53" s="1">
+        <f t="shared" si="3"/>
+        <v>45935.46597222222</v>
+      </c>
+      <c r="C53" s="1">
+        <f t="shared" si="4"/>
+        <v>45935.71597222222</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>278</v>
+      </c>
+      <c r="B54" s="1">
+        <f t="shared" si="3"/>
+        <v>45935.71597222222</v>
+      </c>
+      <c r="C54" s="1">
+        <f t="shared" si="4"/>
+        <v>45935.96597222222</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>279</v>
+      </c>
+      <c r="B55" s="1">
+        <f t="shared" si="3"/>
+        <v>45935.96597222222</v>
+      </c>
+      <c r="C55" s="1">
+        <f t="shared" si="4"/>
+        <v>45936.21597222222</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>280</v>
+      </c>
+      <c r="B56" s="1">
+        <f t="shared" si="3"/>
+        <v>45936.21597222222</v>
+      </c>
+      <c r="C56" s="1">
+        <f t="shared" si="4"/>
+        <v>45936.46597222222</v>
       </c>
     </row>
   </sheetData>
@@ -5425,10 +8312,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A1C8F7-0C5B-6045-992F-0FD6B0162923}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5814,7 +8701,7 @@
         <v>4</v>
       </c>
       <c r="F14">
-        <f t="shared" ref="F14:F37" si="3">(64.069*AVERAGE(D14:D14)-2.8707)*E14</f>
+        <f t="shared" ref="F14:F53" si="3">(64.069*AVERAGE(D14:D14)-2.8707)*E14</f>
         <v>20.807976000000004</v>
       </c>
     </row>
@@ -6161,10 +9048,554 @@
       <c r="F37">
         <f t="shared" si="3"/>
         <v>-0.69235399999999947</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38">
+        <v>0.159</v>
+      </c>
+      <c r="E38">
+        <v>4</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="3"/>
+        <v>29.265084000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C39" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D39">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="3"/>
+        <v>30.802740000000007</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C40" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D40">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="3"/>
+        <v>47.204404000000004</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C41" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D41">
+        <v>0.126</v>
+      </c>
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="3"/>
+        <v>20.807976000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C42" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D42">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="E42">
+        <v>4</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="3"/>
+        <v>205.326696</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C43" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D43">
+        <v>0.79</v>
+      </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+      <c r="F43">
+        <f>(64.069*AVERAGE(D43:D43)-2.8707)*E43</f>
+        <v>190.97524000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C44" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D44">
+        <v>3.1E-2</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="3"/>
+        <v>-0.88456099999999971</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C45" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D45">
+        <v>3.1E-2</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="3"/>
+        <v>-0.88456099999999971</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C46" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D46">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="3"/>
+        <v>29.868559000000005</v>
+      </c>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C47" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D47">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="3"/>
+        <v>28.010558</v>
+      </c>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C48" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D48">
+        <v>0.193</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="3"/>
+        <v>9.4946170000000016</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C49" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D49">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="3"/>
+        <v>15.965586000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C50" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D50">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="3"/>
+        <v>160.47839600000003</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C51" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D51">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="E51">
+        <v>4</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="3"/>
+        <v>140.74514400000001</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C52" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D52">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="3"/>
+        <v>-0.62828499999999954</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C53" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D53">
+        <v>3.1E-2</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="3"/>
+        <v>-0.88456099999999971</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2002340C-AD4C-5C4F-8F00-4A8EC30B67C5}">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" t="s">
+        <v>194</v>
+      </c>
+      <c r="I1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J1" t="s">
+        <v>170</v>
+      </c>
+      <c r="K1" t="s">
+        <v>171</v>
+      </c>
+      <c r="L1" t="s">
+        <v>195</v>
+      </c>
+      <c r="M1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>3.9E-2</v>
+      </c>
+      <c r="G2">
+        <f>AVERAGE(D2:E2)*$K$11 + $K$12</f>
+        <v>-3.2082434215761744</v>
+      </c>
+      <c r="I2">
+        <v>1000</v>
+      </c>
+      <c r="J2">
+        <v>1.556</v>
+      </c>
+      <c r="K2">
+        <v>1.548</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ref="M2:M7" si="0">AVERAGE(J2:L2)</f>
+        <v>1.552</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G13" si="1">AVERAGE(D3:E3)*$K$11 + $K$12</f>
+        <v>8.3261041095816779E-2</v>
+      </c>
+      <c r="I3">
+        <v>500</v>
+      </c>
+      <c r="J3">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="K3">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>0.82450000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>-1.2333407439729775</v>
+      </c>
+      <c r="I4">
+        <v>250</v>
+      </c>
+      <c r="J4">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="K4">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>0.42599999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>-5.1831460991793712</v>
+      </c>
+      <c r="I5">
+        <v>100</v>
+      </c>
+      <c r="J5">
+        <v>0.189</v>
+      </c>
+      <c r="K5">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>0.1915</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>0.04</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>-2.5499425290417754</v>
+      </c>
+      <c r="I6">
+        <v>50</v>
+      </c>
+      <c r="J6">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="K6">
+        <v>0.12</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>0.11899999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D7">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>-4.5248452066449723</v>
+      </c>
+      <c r="I7">
+        <v>25</v>
+      </c>
+      <c r="J7">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="K7">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>7.7499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>2.716464611233409</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K8">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="M8">
+        <f>AVERAGE(J8:L8)</f>
+        <v>5.5999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>8.3261041095816779E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D10">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>1.3998628261646147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>1.3998628261646147</v>
+      </c>
+      <c r="J11" t="s">
+        <v>196</v>
+      </c>
+      <c r="K11">
+        <f>SLOPE(I2:I8,M2:M8)</f>
+        <v>658.30089253439814</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>-4.5248452066449723</v>
+      </c>
+      <c r="K12">
+        <f>INTERCEPT(I2:I8,M2:M8)</f>
+        <v>-28.881978230417701</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>200</v>
+      </c>
+      <c r="D13">
+        <v>0.04</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>-2.5499425290417754</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added good amounts of the tracer experiment data and modelling. Beggining with the new model of the second experiment. TODO: finishi prepare_lab_data_m2.jl among finish the experiment and other details
</commit_message>
<xml_diff>
--- a/data/exp_raw/ssexp_data.xlsx
+++ b/data/exp_raw/ssexp_data.xlsx
@@ -8,20 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vcantarella/Documents/FuhrbergerColumns/data/exp_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7E4A6E-6873-3149-98C9-4726A98149D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78288C1-52D9-6E42-90CD-54AD263614E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="740" windowWidth="28040" windowHeight="16680" xr2:uid="{82067E57-95C1-4A4D-B858-7597035F15DE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="4" xr2:uid="{82067E57-95C1-4A4D-B858-7597035F15DE}"/>
   </bookViews>
   <sheets>
     <sheet name="general_samples_p1" sheetId="1" r:id="rId1"/>
     <sheet name="general_samples_p2" sheetId="4" r:id="rId2"/>
     <sheet name="general_samples_p3" sheetId="5" r:id="rId3"/>
     <sheet name="general_samples_p4" sheetId="6" r:id="rId4"/>
-    <sheet name="fe_total" sheetId="2" r:id="rId5"/>
-    <sheet name="hs" sheetId="3" r:id="rId6"/>
-    <sheet name="standard_curve_no2" sheetId="7" r:id="rId7"/>
-    <sheet name="fe_plate_1" sheetId="8" r:id="rId8"/>
+    <sheet name="bromide_curve" sheetId="9" r:id="rId5"/>
+    <sheet name="fe_total" sheetId="2" r:id="rId6"/>
+    <sheet name="hs" sheetId="3" r:id="rId7"/>
+    <sheet name="standard_curve_no2" sheetId="7" r:id="rId8"/>
+    <sheet name="fe_plate_1" sheetId="8" r:id="rId9"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId10"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="456">
   <si>
     <t>Sample</t>
   </si>
@@ -1204,6 +1208,213 @@
   </si>
   <si>
     <t>intercept:</t>
+  </si>
+  <si>
+    <t>br- [mmol/L]</t>
+  </si>
+  <si>
+    <t>no3- [mgN/L]</t>
+  </si>
+  <si>
+    <t>sample_for_IC</t>
+  </si>
+  <si>
+    <t>B1T1</t>
+  </si>
+  <si>
+    <t>B1T2</t>
+  </si>
+  <si>
+    <t>B1T3</t>
+  </si>
+  <si>
+    <t>B1T4</t>
+  </si>
+  <si>
+    <t>B1T5</t>
+  </si>
+  <si>
+    <t>B1T6</t>
+  </si>
+  <si>
+    <t>B1T7</t>
+  </si>
+  <si>
+    <t>B1T8</t>
+  </si>
+  <si>
+    <t>B1T9</t>
+  </si>
+  <si>
+    <t>B1T10</t>
+  </si>
+  <si>
+    <t>B1T11</t>
+  </si>
+  <si>
+    <t>B1T12</t>
+  </si>
+  <si>
+    <t>B2T1</t>
+  </si>
+  <si>
+    <t>B2T2</t>
+  </si>
+  <si>
+    <t>B2T3</t>
+  </si>
+  <si>
+    <t>B2T4</t>
+  </si>
+  <si>
+    <t>B2T5</t>
+  </si>
+  <si>
+    <t>B2T6</t>
+  </si>
+  <si>
+    <t>B2T7</t>
+  </si>
+  <si>
+    <t>B2T8</t>
+  </si>
+  <si>
+    <t>B2T9</t>
+  </si>
+  <si>
+    <t>B2T10</t>
+  </si>
+  <si>
+    <t>B2T11</t>
+  </si>
+  <si>
+    <t>B2T12</t>
+  </si>
+  <si>
+    <t>B3T1</t>
+  </si>
+  <si>
+    <t>B3T2</t>
+  </si>
+  <si>
+    <t>B3T3</t>
+  </si>
+  <si>
+    <t>B3T4</t>
+  </si>
+  <si>
+    <t>B3T5</t>
+  </si>
+  <si>
+    <t>B3T6</t>
+  </si>
+  <si>
+    <t>B3T7</t>
+  </si>
+  <si>
+    <t>B3T8</t>
+  </si>
+  <si>
+    <t>B3T9</t>
+  </si>
+  <si>
+    <t>B3T10</t>
+  </si>
+  <si>
+    <t>B3T11</t>
+  </si>
+  <si>
+    <t>B3T12</t>
+  </si>
+  <si>
+    <t>B4T1</t>
+  </si>
+  <si>
+    <t>B4T2</t>
+  </si>
+  <si>
+    <t>B4T3</t>
+  </si>
+  <si>
+    <t>B4T4</t>
+  </si>
+  <si>
+    <t>B4T5</t>
+  </si>
+  <si>
+    <t>B4T6</t>
+  </si>
+  <si>
+    <t>B4T7</t>
+  </si>
+  <si>
+    <t>B4T8</t>
+  </si>
+  <si>
+    <t>B4T9</t>
+  </si>
+  <si>
+    <t>B4T10</t>
+  </si>
+  <si>
+    <t>B4T11</t>
+  </si>
+  <si>
+    <t>B4T12</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>end_time</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>volume (ml)</t>
+  </si>
+  <si>
+    <t>concentration mM</t>
+  </si>
+  <si>
+    <t>mass (mg)</t>
+  </si>
+  <si>
+    <t>molar mass</t>
+  </si>
+  <si>
+    <t>stock volume</t>
+  </si>
+  <si>
+    <t>agw volume</t>
+  </si>
+  <si>
+    <t>P1T80</t>
+  </si>
+  <si>
+    <t>P1T81</t>
+  </si>
+  <si>
+    <t>P2T80</t>
+  </si>
+  <si>
+    <t>P2T81</t>
+  </si>
+  <si>
+    <t>P3T80</t>
+  </si>
+  <si>
+    <t>P3T81</t>
+  </si>
+  <si>
+    <t>P4T80</t>
+  </si>
+  <si>
+    <t>P4T81</t>
+  </si>
+  <si>
+    <t>*incomplete</t>
   </si>
 </sst>
 </file>
@@ -1274,6 +1485,410 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Bromide tracer standards</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.10837360847135487"/>
+                  <c:y val="-1.6978189227943952E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-DE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>bromide_curve!$Q$2:$Q$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>166.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>149.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>131.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>113.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36.200000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>bromide_curve!$O$2:$O$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D461-5042-9271-51560FDE2E83}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1081534080"/>
+        <c:axId val="1081535808"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1081534080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1081535808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1081535808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1081534080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -1699,7 +2314,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -2114,7 +2729,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -2610,6 +3225,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4197,7 +4852,566 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>678564</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>16539</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4E8176C-B309-5D44-B036-7E169C2355B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4240,7 +5454,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4283,7 +5497,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4324,6 +5538,83 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="standard_curve_plate_1"/>
+      <sheetName val="standard_curve_plate 2"/>
+      <sheetName val="standard_curve_plate_3"/>
+      <sheetName val="standard_curve_plate 4"/>
+      <sheetName val="fe_plate_1"/>
+      <sheetName val="br_standard_curve"/>
+      <sheetName val="sampling"/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="data"/>
+      <sheetName val="new_data"/>
+      <sheetName val="Sheet2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5">
+        <row r="2">
+          <cell r="L2">
+            <v>1</v>
+          </cell>
+          <cell r="N2">
+            <v>146.80000000000001</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="L3">
+            <v>0.5</v>
+          </cell>
+          <cell r="N3">
+            <v>129.6</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="L4">
+            <v>0.1</v>
+          </cell>
+          <cell r="N4">
+            <v>87.5</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="L5">
+            <v>0.05</v>
+          </cell>
+          <cell r="N5">
+            <v>68.3</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="L6">
+            <v>0.01</v>
+          </cell>
+          <cell r="N6">
+            <v>42.6</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4643,10 +5934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE2E69C-B565-9948-8744-019B7DBC9C60}">
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5949,7 +7240,7 @@
         <v>16.7</v>
       </c>
       <c r="E62">
-        <f t="shared" ref="E62:E68" si="9">(D62-6.75)/6</f>
+        <f t="shared" ref="E62:E82" si="9">(D62-6.75)/6</f>
         <v>1.6583333333333332</v>
       </c>
     </row>
@@ -6103,6 +7394,13 @@
         <f t="shared" si="11"/>
         <v>45939.71597222222</v>
       </c>
+      <c r="D69">
+        <v>18.27</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="9"/>
+        <v>1.92</v>
+      </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
@@ -6116,6 +7414,13 @@
         <f t="shared" si="11"/>
         <v>45939.96597222222</v>
       </c>
+      <c r="D70">
+        <v>18.32</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="9"/>
+        <v>1.9283333333333335</v>
+      </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
@@ -6129,6 +7434,16 @@
         <f t="shared" si="11"/>
         <v>45940.21597222222</v>
       </c>
+      <c r="D71">
+        <v>18.32</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="9"/>
+        <v>1.9283333333333335</v>
+      </c>
+      <c r="H71">
+        <v>9.7200000000000006</v>
+      </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
@@ -6142,6 +7457,13 @@
         <f t="shared" si="11"/>
         <v>45940.46597222222</v>
       </c>
+      <c r="D72">
+        <v>18.37</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="9"/>
+        <v>1.9366666666666668</v>
+      </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
@@ -6155,6 +7477,13 @@
         <f t="shared" si="11"/>
         <v>45940.71597222222</v>
       </c>
+      <c r="D73">
+        <v>17.440000000000001</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="9"/>
+        <v>1.781666666666667</v>
+      </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
@@ -6168,6 +7497,13 @@
         <f t="shared" si="11"/>
         <v>45940.96597222222</v>
       </c>
+      <c r="D74">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="9"/>
+        <v>1.8916666666666668</v>
+      </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
@@ -6181,6 +7517,13 @@
         <f t="shared" si="11"/>
         <v>45941.21597222222</v>
       </c>
+      <c r="D75">
+        <v>18.23</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="9"/>
+        <v>1.9133333333333333</v>
+      </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
@@ -6194,6 +7537,16 @@
         <f t="shared" si="11"/>
         <v>45941.46597222222</v>
       </c>
+      <c r="D76">
+        <v>18.16</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="9"/>
+        <v>1.9016666666666666</v>
+      </c>
+      <c r="H76">
+        <v>9.89</v>
+      </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
@@ -6207,6 +7560,13 @@
         <f t="shared" si="11"/>
         <v>45941.71597222222</v>
       </c>
+      <c r="D77">
+        <v>18.23</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="9"/>
+        <v>1.9133333333333333</v>
+      </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
@@ -6220,6 +7580,13 @@
         <f t="shared" si="11"/>
         <v>45941.96597222222</v>
       </c>
+      <c r="D78">
+        <v>18.190000000000001</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="9"/>
+        <v>1.906666666666667</v>
+      </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
@@ -6233,6 +7600,13 @@
         <f t="shared" si="11"/>
         <v>45942.21597222222</v>
       </c>
+      <c r="D79">
+        <v>18.45</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="9"/>
+        <v>1.95</v>
+      </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
@@ -6245,6 +7619,65 @@
       <c r="C80" s="1">
         <f t="shared" si="11"/>
         <v>45942.46597222222</v>
+      </c>
+      <c r="D80">
+        <v>17.760000000000002</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="9"/>
+        <v>1.8350000000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>447</v>
+      </c>
+      <c r="B81" s="1">
+        <f t="shared" ref="B81:B82" si="12">C80</f>
+        <v>45942.46597222222</v>
+      </c>
+      <c r="C81" s="1">
+        <f t="shared" ref="C81:C82" si="13">B81+6/24</f>
+        <v>45942.71597222222</v>
+      </c>
+      <c r="D81">
+        <v>18.27</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="9"/>
+        <v>1.92</v>
+      </c>
+      <c r="F81">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="G81">
+        <v>715</v>
+      </c>
+      <c r="H81">
+        <v>9.86</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>448</v>
+      </c>
+      <c r="B82" s="1">
+        <f t="shared" si="12"/>
+        <v>45942.71597222222</v>
+      </c>
+      <c r="C82" s="1">
+        <f t="shared" si="13"/>
+        <v>45942.96597222222</v>
+      </c>
+      <c r="D82">
+        <v>13.45</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="9"/>
+        <v>1.1166666666666665</v>
+      </c>
+      <c r="L82" t="s">
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -6255,10 +7688,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046BB4A8-8683-FF42-8F76-0A791D85765F}">
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7317,7 +8750,7 @@
         <v>18.96</v>
       </c>
       <c r="E50">
-        <f t="shared" ref="E50:E68" si="6">(D50-6.75)/6</f>
+        <f t="shared" ref="E50:E82" si="6">(D50-6.75)/6</f>
         <v>2.0350000000000001</v>
       </c>
     </row>
@@ -7725,6 +9158,13 @@
         <f t="shared" si="8"/>
         <v>45939.71597222222</v>
       </c>
+      <c r="D69">
+        <v>18.920000000000002</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="6"/>
+        <v>2.0283333333333338</v>
+      </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
@@ -7738,6 +9178,13 @@
         <f t="shared" si="8"/>
         <v>45939.96597222222</v>
       </c>
+      <c r="D70">
+        <v>18.02</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="6"/>
+        <v>1.8783333333333332</v>
+      </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
@@ -7751,6 +9198,16 @@
         <f t="shared" si="8"/>
         <v>45940.21597222222</v>
       </c>
+      <c r="D71">
+        <v>18.91</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="6"/>
+        <v>2.0266666666666668</v>
+      </c>
+      <c r="H71">
+        <v>7.33</v>
+      </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
@@ -7764,6 +9221,13 @@
         <f t="shared" si="8"/>
         <v>45940.46597222222</v>
       </c>
+      <c r="D72">
+        <v>18.989999999999998</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="6"/>
+        <v>2.0399999999999996</v>
+      </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
@@ -7777,6 +9241,13 @@
         <f t="shared" si="8"/>
         <v>45940.71597222222</v>
       </c>
+      <c r="D73">
+        <v>18.48</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="6"/>
+        <v>1.9550000000000001</v>
+      </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
@@ -7790,6 +9261,13 @@
         <f t="shared" si="8"/>
         <v>45940.96597222222</v>
       </c>
+      <c r="D74">
+        <v>18.850000000000001</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="6"/>
+        <v>2.0166666666666671</v>
+      </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
@@ -7803,6 +9281,13 @@
         <f t="shared" si="8"/>
         <v>45941.21597222222</v>
       </c>
+      <c r="D75">
+        <v>18.53</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="6"/>
+        <v>1.9633333333333336</v>
+      </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
@@ -7816,6 +9301,16 @@
         <f t="shared" si="8"/>
         <v>45941.46597222222</v>
       </c>
+      <c r="D76">
+        <v>18.75</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="H76">
+        <v>7.52</v>
+      </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
@@ -7829,6 +9324,13 @@
         <f t="shared" si="8"/>
         <v>45941.71597222222</v>
       </c>
+      <c r="D77">
+        <v>18.059999999999999</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="6"/>
+        <v>1.8849999999999998</v>
+      </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
@@ -7842,6 +9344,13 @@
         <f t="shared" si="8"/>
         <v>45941.96597222222</v>
       </c>
+      <c r="D78">
+        <v>18.75</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
@@ -7855,6 +9364,13 @@
         <f t="shared" si="8"/>
         <v>45942.21597222222</v>
       </c>
+      <c r="D79">
+        <v>18.89</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="6"/>
+        <v>2.0233333333333334</v>
+      </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
@@ -7867,6 +9383,62 @@
       <c r="C80" s="1">
         <f t="shared" si="8"/>
         <v>45942.46597222222</v>
+      </c>
+      <c r="D80">
+        <v>18.53</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="6"/>
+        <v>1.9633333333333336</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>449</v>
+      </c>
+      <c r="B81" s="1">
+        <f t="shared" ref="B81:B82" si="9">C80</f>
+        <v>45942.46597222222</v>
+      </c>
+      <c r="C81" s="1">
+        <f t="shared" ref="C81:C82" si="10">B81+6/24</f>
+        <v>45942.71597222222</v>
+      </c>
+      <c r="D81">
+        <v>18.89</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="6"/>
+        <v>2.0233333333333334</v>
+      </c>
+      <c r="F81">
+        <v>8.3800000000000008</v>
+      </c>
+      <c r="G81">
+        <v>675</v>
+      </c>
+      <c r="H81">
+        <v>7.54</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>450</v>
+      </c>
+      <c r="B82" s="1">
+        <f t="shared" si="9"/>
+        <v>45942.71597222222</v>
+      </c>
+      <c r="C82" s="1">
+        <f t="shared" si="10"/>
+        <v>45942.96597222222</v>
+      </c>
+      <c r="D82">
+        <v>13.99</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="6"/>
+        <v>1.2066666666666668</v>
       </c>
     </row>
   </sheetData>
@@ -7877,10 +9449,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{649DD004-07E5-F04F-B76F-816E14D1C8AC}">
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7941,7 +9513,7 @@
         <v>17.64</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E68" si="0">(D2-6.75)/6</f>
+        <f t="shared" ref="E2:E82" si="0">(D2-6.75)/6</f>
         <v>1.8150000000000002</v>
       </c>
     </row>
@@ -9368,6 +10940,13 @@
         <f t="shared" si="8"/>
         <v>45939.71597222222</v>
       </c>
+      <c r="D69">
+        <v>18.649999999999999</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="0"/>
+        <v>1.9833333333333332</v>
+      </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
@@ -9381,6 +10960,13 @@
         <f t="shared" si="8"/>
         <v>45939.96597222222</v>
       </c>
+      <c r="D70">
+        <v>19.13</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="0"/>
+        <v>2.063333333333333</v>
+      </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
@@ -9394,6 +10980,16 @@
         <f t="shared" si="8"/>
         <v>45940.21597222222</v>
       </c>
+      <c r="D71">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="0"/>
+        <v>2.0249999999999999</v>
+      </c>
+      <c r="H71">
+        <v>7.87</v>
+      </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
@@ -9407,6 +11003,13 @@
         <f t="shared" si="8"/>
         <v>45940.46597222222</v>
       </c>
+      <c r="D72">
+        <v>18.95</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="0"/>
+        <v>2.0333333333333332</v>
+      </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
@@ -9420,6 +11023,13 @@
         <f t="shared" si="8"/>
         <v>45940.71597222222</v>
       </c>
+      <c r="D73">
+        <v>18.649999999999999</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="0"/>
+        <v>1.9833333333333332</v>
+      </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
@@ -9433,6 +11043,13 @@
         <f t="shared" si="8"/>
         <v>45940.96597222222</v>
       </c>
+      <c r="D74">
+        <v>18.73</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="0"/>
+        <v>1.9966666666666668</v>
+      </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
@@ -9446,6 +11063,13 @@
         <f t="shared" si="8"/>
         <v>45941.21597222222</v>
       </c>
+      <c r="D75">
+        <v>17.71</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="0"/>
+        <v>1.8266666666666669</v>
+      </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
@@ -9459,6 +11083,16 @@
         <f t="shared" si="8"/>
         <v>45941.46597222222</v>
       </c>
+      <c r="D76">
+        <v>18.77</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="0"/>
+        <v>2.0033333333333334</v>
+      </c>
+      <c r="H76">
+        <v>8.76</v>
+      </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
@@ -9472,6 +11106,13 @@
         <f t="shared" si="8"/>
         <v>45941.71597222222</v>
       </c>
+      <c r="D77">
+        <v>18.920000000000002</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="0"/>
+        <v>2.0283333333333338</v>
+      </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
@@ -9485,6 +11126,13 @@
         <f t="shared" si="8"/>
         <v>45941.96597222222</v>
       </c>
+      <c r="D78">
+        <v>18.68</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="0"/>
+        <v>1.9883333333333333</v>
+      </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
@@ -9498,6 +11146,13 @@
         <f t="shared" si="8"/>
         <v>45942.21597222222</v>
       </c>
+      <c r="D79">
+        <v>18.77</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="0"/>
+        <v>2.0033333333333334</v>
+      </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
@@ -9510,6 +11165,62 @@
       <c r="C80" s="1">
         <f t="shared" si="8"/>
         <v>45942.46597222222</v>
+      </c>
+      <c r="D80">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="0"/>
+        <v>1.968333333333333</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>451</v>
+      </c>
+      <c r="B81" s="1">
+        <f t="shared" ref="B81:B82" si="9">C80</f>
+        <v>45942.46597222222</v>
+      </c>
+      <c r="C81" s="1">
+        <f t="shared" ref="C81:C82" si="10">B81+6/24</f>
+        <v>45942.71597222222</v>
+      </c>
+      <c r="D81">
+        <v>18.61</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="0"/>
+        <v>1.9766666666666666</v>
+      </c>
+      <c r="F81">
+        <v>7.98</v>
+      </c>
+      <c r="G81">
+        <v>729</v>
+      </c>
+      <c r="H81">
+        <v>8.44</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>452</v>
+      </c>
+      <c r="B82" s="1">
+        <f t="shared" si="9"/>
+        <v>45942.71597222222</v>
+      </c>
+      <c r="C82" s="1">
+        <f t="shared" si="10"/>
+        <v>45942.96597222222</v>
+      </c>
+      <c r="D82">
+        <v>14</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="0"/>
+        <v>1.2083333333333333</v>
       </c>
     </row>
   </sheetData>
@@ -9520,10 +11231,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CEAE0A4-BA85-AC4B-952F-A9D4082FC119}">
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G81" sqref="G81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10833,7 +12544,7 @@
         <v>17.829999999999998</v>
       </c>
       <c r="E63">
-        <f t="shared" ref="E63:E68" si="9">(D63-6.75)/6</f>
+        <f t="shared" ref="E63:E82" si="9">(D63-6.75)/6</f>
         <v>1.8466666666666665</v>
       </c>
     </row>
@@ -10961,6 +12672,13 @@
         <f t="shared" si="6"/>
         <v>45939.71597222222</v>
       </c>
+      <c r="D69">
+        <v>18.61</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="9"/>
+        <v>1.9766666666666666</v>
+      </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
@@ -10974,6 +12692,13 @@
         <f t="shared" si="6"/>
         <v>45939.96597222222</v>
       </c>
+      <c r="D70">
+        <v>18.579999999999998</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="9"/>
+        <v>1.9716666666666665</v>
+      </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
@@ -10987,6 +12712,13 @@
         <f t="shared" si="6"/>
         <v>45940.21597222222</v>
       </c>
+      <c r="D71">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="9"/>
+        <v>1.9750000000000003</v>
+      </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
@@ -11000,6 +12732,13 @@
         <f t="shared" si="6"/>
         <v>45940.46597222222</v>
       </c>
+      <c r="D72">
+        <v>18.77</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="9"/>
+        <v>2.0033333333333334</v>
+      </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
@@ -11013,6 +12752,13 @@
         <f t="shared" si="6"/>
         <v>45940.71597222222</v>
       </c>
+      <c r="D73">
+        <v>18.809999999999999</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="9"/>
+        <v>2.0099999999999998</v>
+      </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
@@ -11026,6 +12772,13 @@
         <f t="shared" si="6"/>
         <v>45940.96597222222</v>
       </c>
+      <c r="D74">
+        <v>18.440000000000001</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="9"/>
+        <v>1.9483333333333335</v>
+      </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
@@ -11039,6 +12792,13 @@
         <f t="shared" si="6"/>
         <v>45941.21597222222</v>
       </c>
+      <c r="D75">
+        <v>18.5</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="9"/>
+        <v>1.9583333333333333</v>
+      </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
@@ -11052,6 +12812,13 @@
         <f t="shared" si="6"/>
         <v>45941.46597222222</v>
       </c>
+      <c r="D76">
+        <v>18.489999999999998</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="9"/>
+        <v>1.9566666666666663</v>
+      </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
@@ -11065,6 +12832,13 @@
         <f t="shared" si="6"/>
         <v>45941.71597222222</v>
       </c>
+      <c r="D77">
+        <v>18.510000000000002</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="9"/>
+        <v>1.9600000000000002</v>
+      </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
@@ -11078,6 +12852,13 @@
         <f t="shared" si="6"/>
         <v>45941.96597222222</v>
       </c>
+      <c r="D78">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="9"/>
+        <v>1.968333333333333</v>
+      </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
@@ -11091,6 +12872,13 @@
         <f t="shared" si="6"/>
         <v>45942.21597222222</v>
       </c>
+      <c r="D79">
+        <v>18.579999999999998</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="9"/>
+        <v>1.9716666666666665</v>
+      </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
@@ -11103,6 +12891,59 @@
       <c r="C80" s="1">
         <f t="shared" si="6"/>
         <v>45942.46597222222</v>
+      </c>
+      <c r="D80">
+        <v>18.579999999999998</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="9"/>
+        <v>1.9716666666666665</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>453</v>
+      </c>
+      <c r="B81" s="1">
+        <f t="shared" ref="B81:B82" si="10">C80</f>
+        <v>45942.46597222222</v>
+      </c>
+      <c r="C81" s="1">
+        <f t="shared" ref="C81:C82" si="11">B81+6/24</f>
+        <v>45942.71597222222</v>
+      </c>
+      <c r="D81">
+        <v>18.57</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="9"/>
+        <v>1.97</v>
+      </c>
+      <c r="F81">
+        <v>8.06</v>
+      </c>
+      <c r="G81">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>454</v>
+      </c>
+      <c r="B82" s="1">
+        <f t="shared" si="10"/>
+        <v>45942.71597222222</v>
+      </c>
+      <c r="C82" s="1">
+        <f t="shared" si="11"/>
+        <v>45942.96597222222</v>
+      </c>
+      <c r="D82">
+        <v>13.74</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="9"/>
+        <v>1.165</v>
       </c>
     </row>
   </sheetData>
@@ -11112,6 +12953,1500 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613850BE-EF2F-F44E-9131-45DE0F67BB0D}">
+  <dimension ref="A1:Z49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8" customWidth="1"/>
+    <col min="24" max="24" width="10.33203125" customWidth="1"/>
+    <col min="25" max="25" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D1" t="s">
+        <v>440</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1" t="s">
+        <v>388</v>
+      </c>
+      <c r="I1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J1" t="s">
+        <v>389</v>
+      </c>
+      <c r="O1" t="s">
+        <v>168</v>
+      </c>
+      <c r="P1" t="s">
+        <v>169</v>
+      </c>
+      <c r="U1" t="s">
+        <v>442</v>
+      </c>
+      <c r="V1" t="s">
+        <v>441</v>
+      </c>
+      <c r="W1" t="s">
+        <v>443</v>
+      </c>
+      <c r="X1" t="s">
+        <v>444</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>445</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="19" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45942.886111111111</v>
+      </c>
+      <c r="C2" s="1">
+        <f>B2+2/24</f>
+        <v>45942.969444444447</v>
+      </c>
+      <c r="D2">
+        <v>10.65</v>
+      </c>
+      <c r="E2">
+        <f>(D2-6.75)/2</f>
+        <v>1.9500000000000002</v>
+      </c>
+      <c r="F2">
+        <v>-33.5</v>
+      </c>
+      <c r="G2">
+        <f>0.0076*EXP(0.0328*-F2)</f>
+        <v>2.2804280220077435E-2</v>
+      </c>
+      <c r="H2">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>-166.7</v>
+      </c>
+      <c r="Q2">
+        <f>-1*P2</f>
+        <v>166.7</v>
+      </c>
+      <c r="U2">
+        <v>10</v>
+      </c>
+      <c r="V2">
+        <v>50</v>
+      </c>
+      <c r="W2">
+        <f>X2*U2*V2/1000</f>
+        <v>51.445000000000007</v>
+      </c>
+      <c r="X2">
+        <v>102.89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>391</v>
+      </c>
+      <c r="B3" s="1">
+        <f>C2</f>
+        <v>45942.969444444447</v>
+      </c>
+      <c r="C3" s="1">
+        <f>B3+2/24</f>
+        <v>45943.052777777782</v>
+      </c>
+      <c r="D3">
+        <v>10.55</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E49" si="0">(D3-6.75)/2</f>
+        <v>1.9000000000000004</v>
+      </c>
+      <c r="F3">
+        <v>-34.299999999999997</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G49" si="1">0.0076*EXP(0.0328*-F3)</f>
+        <v>2.3410584456427078E-2</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>-149.19999999999999</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q8" si="2">-1*P3</f>
+        <v>149.19999999999999</v>
+      </c>
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="V3">
+        <v>8</v>
+      </c>
+      <c r="Y3">
+        <f>U3/U2*V3</f>
+        <v>1.6</v>
+      </c>
+      <c r="Z3">
+        <f>V3-Y3</f>
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" ref="B4:B13" si="3">C3</f>
+        <v>45943.052777777782</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ref="C4:C13" si="4">B4+2/24</f>
+        <v>45943.136111111118</v>
+      </c>
+      <c r="D4">
+        <v>10.56</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>1.9050000000000002</v>
+      </c>
+      <c r="F4">
+        <v>-34.4</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>2.3487497241456743E-2</v>
+      </c>
+      <c r="O4">
+        <v>0.5</v>
+      </c>
+      <c r="P4">
+        <v>-131.19999999999999</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="2"/>
+        <v>131.19999999999999</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>8</v>
+      </c>
+      <c r="Y4">
+        <f>U4/$U$2*V4</f>
+        <v>0.8</v>
+      </c>
+      <c r="Z4">
+        <f>V4-Y4</f>
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="3"/>
+        <v>45943.136111111118</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="4"/>
+        <v>45943.219444444454</v>
+      </c>
+      <c r="D5">
+        <v>10.64</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>1.9450000000000003</v>
+      </c>
+      <c r="F5">
+        <v>-70</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>7.5501177132492991E-2</v>
+      </c>
+      <c r="O5">
+        <v>0.25</v>
+      </c>
+      <c r="P5">
+        <v>-113.3</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="2"/>
+        <v>113.3</v>
+      </c>
+      <c r="U5">
+        <v>0.5</v>
+      </c>
+      <c r="V5">
+        <v>8</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" ref="Y5:Y7" si="5">U5/$U$2*V5</f>
+        <v>0.4</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" ref="Z5:Z7" si="6">V5-Y5</f>
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>394</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="3"/>
+        <v>45943.219444444454</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="4"/>
+        <v>45943.30277777779</v>
+      </c>
+      <c r="D6">
+        <v>10.61</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>1.9299999999999997</v>
+      </c>
+      <c r="F6">
+        <v>-122.8</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>0.42666034310679996</v>
+      </c>
+      <c r="H6">
+        <v>4.49</v>
+      </c>
+      <c r="O6">
+        <v>0.1</v>
+      </c>
+      <c r="P6">
+        <v>-57.4</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="2"/>
+        <v>57.4</v>
+      </c>
+      <c r="U6">
+        <v>0.25</v>
+      </c>
+      <c r="V6">
+        <v>8</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="5"/>
+        <v>0.2</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="6"/>
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>395</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="3"/>
+        <v>45943.30277777779</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="4"/>
+        <v>45943.386111111126</v>
+      </c>
+      <c r="D7">
+        <v>10.57</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>1.9100000000000001</v>
+      </c>
+      <c r="F7">
+        <v>-136.19999999999999</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0.66216068117437099</v>
+      </c>
+      <c r="O7">
+        <v>0.05</v>
+      </c>
+      <c r="P7">
+        <v>-42.5</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="2"/>
+        <v>42.5</v>
+      </c>
+      <c r="U7">
+        <v>0.1</v>
+      </c>
+      <c r="V7">
+        <v>4</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="5"/>
+        <v>0.04</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="6"/>
+        <v>3.96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>396</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="3"/>
+        <v>45943.386111111126</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="4"/>
+        <v>45943.469444444461</v>
+      </c>
+      <c r="D8">
+        <v>10.63</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1.9400000000000004</v>
+      </c>
+      <c r="F8">
+        <v>-141.19999999999999</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>0.78016719345119157</v>
+      </c>
+      <c r="O8">
+        <v>0.01</v>
+      </c>
+      <c r="P8">
+        <v>-36.200000000000003</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="2"/>
+        <v>36.200000000000003</v>
+      </c>
+      <c r="Y8">
+        <f>SUM(Y3:Y7)</f>
+        <v>3.0400000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>397</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="3"/>
+        <v>45943.469444444461</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="4"/>
+        <v>45943.552777777797</v>
+      </c>
+      <c r="D9">
+        <v>10.57</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>1.9100000000000001</v>
+      </c>
+      <c r="F9">
+        <v>-141.6</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0.79047042845623094</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>398</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="3"/>
+        <v>45943.552777777797</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="4"/>
+        <v>45943.636111111133</v>
+      </c>
+      <c r="D10">
+        <v>10.58</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>1.915</v>
+      </c>
+      <c r="F10">
+        <v>-142.69999999999999</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0.81951134942292403</v>
+      </c>
+      <c r="H10">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>399</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="3"/>
+        <v>45943.636111111133</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="4"/>
+        <v>45943.719444444469</v>
+      </c>
+      <c r="D11">
+        <v>10.71</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>1.9800000000000004</v>
+      </c>
+      <c r="F11">
+        <v>-143.19999999999999</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0.83306214838775894</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>400</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="3"/>
+        <v>45943.719444444469</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="4"/>
+        <v>45943.802777777804</v>
+      </c>
+      <c r="D12">
+        <v>10.54</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>1.8949999999999996</v>
+      </c>
+      <c r="F12">
+        <f>-143-2</f>
+        <v>-145</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0.88372704938254254</v>
+      </c>
+      <c r="H12">
+        <v>1.72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>401</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="3"/>
+        <v>45943.802777777804</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="4"/>
+        <v>45943.88611111114</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>7.6E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>402</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45942.886111111111</v>
+      </c>
+      <c r="C14" s="1">
+        <f>B14+2/24</f>
+        <v>45942.969444444447</v>
+      </c>
+      <c r="D14">
+        <v>10.67</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>1.96</v>
+      </c>
+      <c r="F14">
+        <v>-40.6</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>2.8784246682358017E-2</v>
+      </c>
+      <c r="H14">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>403</v>
+      </c>
+      <c r="B15" s="1">
+        <f>C14</f>
+        <v>45942.969444444447</v>
+      </c>
+      <c r="C15" s="1">
+        <f>B15+2/24</f>
+        <v>45943.052777777782</v>
+      </c>
+      <c r="D15">
+        <v>11.05</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>2.1500000000000004</v>
+      </c>
+      <c r="F15">
+        <v>-40.200000000000003</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>2.8409063946438932E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>404</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" ref="B16:B25" si="7">C15</f>
+        <v>45943.052777777782</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" ref="C16:C25" si="8">B16+2/24</f>
+        <v>45943.136111111118</v>
+      </c>
+      <c r="D16">
+        <v>10.63</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>1.9400000000000004</v>
+      </c>
+      <c r="F16">
+        <v>-55.4</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>4.6771228923828782E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>405</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="7"/>
+        <v>45943.136111111118</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="8"/>
+        <v>45943.219444444454</v>
+      </c>
+      <c r="D17">
+        <v>10.8</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>2.0250000000000004</v>
+      </c>
+      <c r="F17">
+        <v>-104.9</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>0.23719159856480895</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>406</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="7"/>
+        <v>45943.219444444454</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="8"/>
+        <v>45943.30277777779</v>
+      </c>
+      <c r="D18">
+        <v>10.66</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>1.9550000000000001</v>
+      </c>
+      <c r="F18">
+        <v>-131.4</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>0.56570245793969465</v>
+      </c>
+      <c r="H18">
+        <v>2.3199999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>407</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" si="7"/>
+        <v>45943.30277777779</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="8"/>
+        <v>45943.386111111126</v>
+      </c>
+      <c r="D19">
+        <v>10.83</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>2.04</v>
+      </c>
+      <c r="F19">
+        <v>-136.69999999999999</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>0.67310965250872823</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>408</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="7"/>
+        <v>45943.386111111126</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="8"/>
+        <v>45943.469444444461</v>
+      </c>
+      <c r="D20">
+        <v>10.88</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>2.0650000000000004</v>
+      </c>
+      <c r="F20">
+        <v>-141.6</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>0.79047042845623094</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>409</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="7"/>
+        <v>45943.469444444461</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="8"/>
+        <v>45943.552777777797</v>
+      </c>
+      <c r="D21">
+        <v>10.63</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>1.9400000000000004</v>
+      </c>
+      <c r="F21">
+        <v>-143.80000000000001</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>0.84961919846210943</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>410</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="7"/>
+        <v>45943.552777777797</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="8"/>
+        <v>45943.636111111133</v>
+      </c>
+      <c r="D22">
+        <v>9.5</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>1.375</v>
+      </c>
+      <c r="F22">
+        <v>-145.80000000000001</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>0.90722296544068992</v>
+      </c>
+      <c r="H22">
+        <v>0.86799999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>411</v>
+      </c>
+      <c r="B23" s="1">
+        <f t="shared" si="7"/>
+        <v>45943.636111111133</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="8"/>
+        <v>45943.719444444469</v>
+      </c>
+      <c r="D23">
+        <v>11.24</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>2.2450000000000001</v>
+      </c>
+      <c r="F23">
+        <v>-145.69999999999999</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>0.90425214891657868</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>412</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" si="7"/>
+        <v>45943.719444444469</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="8"/>
+        <v>45943.802777777804</v>
+      </c>
+      <c r="D24">
+        <v>10.76</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="F24">
+        <v>-144.19999999999999</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>0.86083964754023978</v>
+      </c>
+      <c r="H24">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>413</v>
+      </c>
+      <c r="B25" s="1">
+        <f t="shared" si="7"/>
+        <v>45943.802777777804</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="8"/>
+        <v>45943.88611111114</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>7.6E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>414</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45942.886111111111</v>
+      </c>
+      <c r="C26" s="1">
+        <f>B26+2/24</f>
+        <v>45942.969444444447</v>
+      </c>
+      <c r="D26">
+        <v>10.81</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>2.0300000000000002</v>
+      </c>
+      <c r="F26">
+        <v>-43.4</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>3.1552986610876278E-2</v>
+      </c>
+      <c r="H26">
+        <v>8.42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>415</v>
+      </c>
+      <c r="B27" s="1">
+        <f>C26</f>
+        <v>45942.969444444447</v>
+      </c>
+      <c r="C27" s="1">
+        <f>B27+2/24</f>
+        <v>45943.052777777782</v>
+      </c>
+      <c r="D27">
+        <v>10.67</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>1.96</v>
+      </c>
+      <c r="F27">
+        <v>-46.9</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>3.5391378571216117E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>416</v>
+      </c>
+      <c r="B28" s="1">
+        <f t="shared" ref="B28:B37" si="9">C27</f>
+        <v>45943.052777777782</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" ref="C28:C37" si="10">B28+2/24</f>
+        <v>45943.136111111118</v>
+      </c>
+      <c r="D28">
+        <v>10.8</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>2.0250000000000004</v>
+      </c>
+      <c r="F28">
+        <v>-59.9</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>5.4210154716647078E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>417</v>
+      </c>
+      <c r="B29" s="1">
+        <f t="shared" si="9"/>
+        <v>45943.136111111118</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="10"/>
+        <v>45943.219444444454</v>
+      </c>
+      <c r="D29">
+        <v>10.83</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>2.04</v>
+      </c>
+      <c r="F29">
+        <v>-107.7</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>0.26000692032405337</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>418</v>
+      </c>
+      <c r="B30" s="1">
+        <f t="shared" si="9"/>
+        <v>45943.219444444454</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="10"/>
+        <v>45943.30277777779</v>
+      </c>
+      <c r="D30">
+        <v>10.78</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>2.0149999999999997</v>
+      </c>
+      <c r="F30">
+        <v>-133.6</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>0.60803244698404435</v>
+      </c>
+      <c r="H30">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>419</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="9"/>
+        <v>45943.30277777779</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="10"/>
+        <v>45943.386111111126</v>
+      </c>
+      <c r="D31">
+        <v>10.66</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>1.9550000000000001</v>
+      </c>
+      <c r="F31">
+        <v>-139.1</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>0.72823823991541325</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>420</v>
+      </c>
+      <c r="B32" s="1">
+        <f t="shared" si="9"/>
+        <v>45943.386111111126</v>
+      </c>
+      <c r="C32" s="1">
+        <f t="shared" si="10"/>
+        <v>45943.469444444461</v>
+      </c>
+      <c r="D32">
+        <v>10.83</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>2.04</v>
+      </c>
+      <c r="F32">
+        <v>-141.6</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>0.79047042845623094</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>421</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" si="9"/>
+        <v>45943.469444444461</v>
+      </c>
+      <c r="C33" s="1">
+        <f t="shared" si="10"/>
+        <v>45943.552777777797</v>
+      </c>
+      <c r="D33">
+        <v>10.67</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>1.96</v>
+      </c>
+      <c r="F33">
+        <v>-144.1</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>0.85802071906626864</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>422</v>
+      </c>
+      <c r="B34" s="1">
+        <f t="shared" si="9"/>
+        <v>45943.552777777797</v>
+      </c>
+      <c r="C34" s="1">
+        <f t="shared" si="10"/>
+        <v>45943.636111111133</v>
+      </c>
+      <c r="D34">
+        <v>10.7</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>1.9749999999999996</v>
+      </c>
+      <c r="F34">
+        <v>-146.5</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>0.92829377195073626</v>
+      </c>
+      <c r="H34">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>423</v>
+      </c>
+      <c r="B35" s="1">
+        <f t="shared" si="9"/>
+        <v>45943.636111111133</v>
+      </c>
+      <c r="C35" s="1">
+        <f t="shared" si="10"/>
+        <v>45943.719444444469</v>
+      </c>
+      <c r="D35">
+        <v>9.98</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>1.6150000000000002</v>
+      </c>
+      <c r="F35">
+        <v>-146</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>0.91319391138408179</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>424</v>
+      </c>
+      <c r="B36" s="1">
+        <f t="shared" si="9"/>
+        <v>45943.719444444469</v>
+      </c>
+      <c r="C36" s="1">
+        <f t="shared" si="10"/>
+        <v>45943.802777777804</v>
+      </c>
+      <c r="D36">
+        <v>10.95</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>2.0999999999999996</v>
+      </c>
+      <c r="F36">
+        <v>-144.5</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>0.86935212236281723</v>
+      </c>
+      <c r="H36">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>425</v>
+      </c>
+      <c r="B37" s="1">
+        <f t="shared" si="9"/>
+        <v>45943.802777777804</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" si="10"/>
+        <v>45943.88611111114</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>7.6E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>426</v>
+      </c>
+      <c r="B38" s="1">
+        <v>45942.886111111111</v>
+      </c>
+      <c r="C38" s="1">
+        <f>B38+2/24</f>
+        <v>45942.969444444447</v>
+      </c>
+      <c r="D38">
+        <v>10.64</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>1.9450000000000003</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>7.6E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>427</v>
+      </c>
+      <c r="B39" s="1">
+        <f>C38</f>
+        <v>45942.969444444447</v>
+      </c>
+      <c r="C39" s="1">
+        <f>B39+2/24</f>
+        <v>45943.052777777782</v>
+      </c>
+      <c r="D39">
+        <v>10.68</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>1.9649999999999999</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>7.6E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>428</v>
+      </c>
+      <c r="B40" s="1">
+        <f t="shared" ref="B40:B49" si="11">C39</f>
+        <v>45943.052777777782</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" ref="C40:C49" si="12">B40+2/24</f>
+        <v>45943.136111111118</v>
+      </c>
+      <c r="D40">
+        <v>10.68</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>1.9649999999999999</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>7.6E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>429</v>
+      </c>
+      <c r="B41" s="1">
+        <f t="shared" si="11"/>
+        <v>45943.136111111118</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" si="12"/>
+        <v>45943.219444444454</v>
+      </c>
+      <c r="D41">
+        <v>10.76</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>7.6E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>430</v>
+      </c>
+      <c r="B42" s="1">
+        <f t="shared" si="11"/>
+        <v>45943.219444444454</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" si="12"/>
+        <v>45943.30277777779</v>
+      </c>
+      <c r="D42">
+        <v>10.67</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>1.96</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>7.6E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>431</v>
+      </c>
+      <c r="B43" s="1">
+        <f t="shared" si="11"/>
+        <v>45943.30277777779</v>
+      </c>
+      <c r="C43" s="1">
+        <f t="shared" si="12"/>
+        <v>45943.386111111126</v>
+      </c>
+      <c r="D43">
+        <v>10.66</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>1.9550000000000001</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>7.6E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>432</v>
+      </c>
+      <c r="B44" s="1">
+        <f t="shared" si="11"/>
+        <v>45943.386111111126</v>
+      </c>
+      <c r="C44" s="1">
+        <f t="shared" si="12"/>
+        <v>45943.469444444461</v>
+      </c>
+      <c r="D44">
+        <v>10.73</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>1.9900000000000002</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>7.6E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>433</v>
+      </c>
+      <c r="B45" s="1">
+        <f t="shared" si="11"/>
+        <v>45943.469444444461</v>
+      </c>
+      <c r="C45" s="1">
+        <f t="shared" si="12"/>
+        <v>45943.552777777797</v>
+      </c>
+      <c r="D45">
+        <v>10.64</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>1.9450000000000003</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>7.6E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>434</v>
+      </c>
+      <c r="B46" s="1">
+        <f t="shared" si="11"/>
+        <v>45943.552777777797</v>
+      </c>
+      <c r="C46" s="1">
+        <f t="shared" si="12"/>
+        <v>45943.636111111133</v>
+      </c>
+      <c r="D46">
+        <v>10.71</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>1.9800000000000004</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="1"/>
+        <v>7.6E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>435</v>
+      </c>
+      <c r="B47" s="1">
+        <f t="shared" si="11"/>
+        <v>45943.636111111133</v>
+      </c>
+      <c r="C47" s="1">
+        <f t="shared" si="12"/>
+        <v>45943.719444444469</v>
+      </c>
+      <c r="D47">
+        <v>10.69</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>1.9699999999999998</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="1"/>
+        <v>7.6E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>436</v>
+      </c>
+      <c r="B48" s="1">
+        <f t="shared" si="11"/>
+        <v>45943.719444444469</v>
+      </c>
+      <c r="C48" s="1">
+        <f t="shared" si="12"/>
+        <v>45943.802777777804</v>
+      </c>
+      <c r="D48">
+        <v>10.66</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>1.9550000000000001</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="1"/>
+        <v>7.6E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>437</v>
+      </c>
+      <c r="B49" s="1">
+        <f t="shared" si="11"/>
+        <v>45943.802777777804</v>
+      </c>
+      <c r="C49" s="1">
+        <f t="shared" si="12"/>
+        <v>45943.88611111114</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="1"/>
+        <v>7.6E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16994493-3AAA-0649-9876-DE782407159B}">
   <dimension ref="A1:L17"/>
   <sheetViews>
@@ -11472,7 +14807,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5BDF59F-AB87-404D-AFD3-7683E8E88CAC}">
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -11513,12 +14848,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A1C8F7-0C5B-6045-992F-0FD6B0162923}">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView zoomScale="118" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView topLeftCell="A36" zoomScale="118" workbookViewId="0">
+      <selection activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12746,7 +16081,7 @@
         <v>1</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F69" si="3">($J$11*AVERAGE(D67:D67)+$J$12)*E67</f>
+        <f t="shared" ref="F67:F81" si="3">($J$11*AVERAGE(D67:D67)+$J$12)*E67</f>
         <v>35.273579856115113</v>
       </c>
     </row>
@@ -12778,6 +16113,186 @@
       <c r="F69">
         <f t="shared" si="3"/>
         <v>-0.71290071942446454</v>
+      </c>
+    </row>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C70" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D70">
+        <v>0.48</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="3"/>
+        <v>25.806548201438847</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C71" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D71">
+        <v>0.504</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="3"/>
+        <v>27.21778273381295</v>
+      </c>
+    </row>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C72" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="D72">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="3"/>
+        <v>27.982201438848922</v>
+      </c>
+    </row>
+    <row r="73" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C73" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D73">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="3"/>
+        <v>37.860843165467635</v>
+      </c>
+    </row>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C74" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D74">
+        <v>0.72</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="3"/>
+        <v>39.918893525179861</v>
+      </c>
+    </row>
+    <row r="75" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C75" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D75">
+        <v>0.746</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="3"/>
+        <v>41.447730935251805</v>
+      </c>
+    </row>
+    <row r="76" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C76" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D76">
+        <v>0.313</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="3"/>
+        <v>15.986707913669065</v>
+      </c>
+    </row>
+    <row r="77" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C77" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D77">
+        <v>0.253</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="3"/>
+        <v>12.45862158273381</v>
+      </c>
+    </row>
+    <row r="78" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C78" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="D78">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="3"/>
+        <v>11.811805755395682</v>
+      </c>
+    </row>
+    <row r="79" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C79" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="D79">
+        <v>3.1E-2</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="3"/>
+        <v>-0.59529784172662281</v>
+      </c>
+    </row>
+    <row r="80" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C80" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="D80">
+        <v>3.1E-2</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="3"/>
+        <v>-0.59529784172662281</v>
+      </c>
+    </row>
+    <row r="81" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C81" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="D81">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="3"/>
+        <v>-0.18368776978417678</v>
       </c>
     </row>
   </sheetData>
@@ -12787,7 +16302,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2002340C-AD4C-5C4F-8F00-4A8EC30B67C5}">
   <dimension ref="A1:M13"/>
   <sheetViews>

</xml_diff>